<commit_message>
Made table more readable by adding predicted salaries
</commit_message>
<xml_diff>
--- a/residualTable.xlsx
+++ b/residualTable.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C434"/>
+  <dimension ref="A1:D434"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,6 +370,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Predicted Salary</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Residual</t>
         </is>
       </c>
@@ -384,6 +389,9 @@
         <v>4379527</v>
       </c>
       <c r="C2">
+        <v>3899514.690630183</v>
+      </c>
+      <c r="D2">
         <v>480012.3093698169</v>
       </c>
     </row>
@@ -397,6 +405,9 @@
         <v>32600060</v>
       </c>
       <c r="C3">
+        <v>31900849.80273632</v>
+      </c>
+      <c r="D3">
         <v>699210.1972636804</v>
       </c>
     </row>
@@ -410,6 +421,9 @@
         <v>4114200</v>
       </c>
       <c r="C4">
+        <v>3553369.743449421</v>
+      </c>
+      <c r="D4">
         <v>560830.2565505793</v>
       </c>
     </row>
@@ -423,6 +437,9 @@
         <v>2194200</v>
       </c>
       <c r="C5">
+        <v>7444835.821227196</v>
+      </c>
+      <c r="D5">
         <v>-5250635.821227196</v>
       </c>
     </row>
@@ -436,6 +453,9 @@
         <v>4687500</v>
       </c>
       <c r="C6">
+        <v>3980186.416915425</v>
+      </c>
+      <c r="D6">
         <v>707313.5830845754</v>
       </c>
     </row>
@@ -449,6 +469,9 @@
         <v>8925000</v>
       </c>
       <c r="C7">
+        <v>15808175.85016584</v>
+      </c>
+      <c r="D7">
         <v>-6883175.850165844</v>
       </c>
     </row>
@@ -462,6 +485,9 @@
         <v>20000000</v>
       </c>
       <c r="C8">
+        <v>19299054.41666666</v>
+      </c>
+      <c r="D8">
         <v>700945.5833333395</v>
       </c>
     </row>
@@ -475,6 +501,9 @@
         <v>1836096</v>
       </c>
       <c r="C9">
+        <v>2704563.414262024</v>
+      </c>
+      <c r="D9">
         <v>-868467.4142620238</v>
       </c>
     </row>
@@ -488,6 +517,9 @@
         <v>9219512</v>
       </c>
       <c r="C10">
+        <v>10737768.80588723</v>
+      </c>
+      <c r="D10">
         <v>-1518256.80588723</v>
       </c>
     </row>
@@ -501,6 +533,9 @@
         <v>45640084</v>
       </c>
       <c r="C11">
+        <v>42212862.49900497</v>
+      </c>
+      <c r="D11">
         <v>3427221.500995025</v>
       </c>
     </row>
@@ -514,6 +549,9 @@
         <v>2019706</v>
       </c>
       <c r="C12">
+        <v>3061282.498590381</v>
+      </c>
+      <c r="D12">
         <v>-1041576.498590381</v>
       </c>
     </row>
@@ -527,6 +565,9 @@
         <v>5539771</v>
       </c>
       <c r="C13">
+        <v>7333060.723714761</v>
+      </c>
+      <c r="D13">
         <v>-1793289.723714761</v>
       </c>
     </row>
@@ -540,6 +581,9 @@
         <v>18642857</v>
       </c>
       <c r="C14">
+        <v>18731746.55232173</v>
+      </c>
+      <c r="D14">
         <v>-88889.55232173204</v>
       </c>
     </row>
@@ -553,6 +597,9 @@
         <v>2019706</v>
       </c>
       <c r="C15">
+        <v>2171512.623466004</v>
+      </c>
+      <c r="D15">
         <v>-151806.6234660042</v>
       </c>
     </row>
@@ -566,6 +613,9 @@
         <v>6263188</v>
       </c>
       <c r="C16">
+        <v>7681002.686567168</v>
+      </c>
+      <c r="D16">
         <v>-1417814.686567168</v>
       </c>
     </row>
@@ -579,6 +629,9 @@
         <v>32459438</v>
       </c>
       <c r="C17">
+        <v>25937187.58009949</v>
+      </c>
+      <c r="D17">
         <v>6522250.419900507</v>
       </c>
     </row>
@@ -592,6 +645,9 @@
         <v>12500000</v>
       </c>
       <c r="C18">
+        <v>9050280.198673299</v>
+      </c>
+      <c r="D18">
         <v>3449719.801326701</v>
       </c>
     </row>
@@ -605,6 +661,9 @@
         <v>2337720</v>
       </c>
       <c r="C19">
+        <v>2632173.396351576</v>
+      </c>
+      <c r="D19">
         <v>-294453.3963515759</v>
       </c>
     </row>
@@ -618,6 +677,9 @@
         <v>10900635</v>
       </c>
       <c r="C20">
+        <v>13888908.48341626</v>
+      </c>
+      <c r="D20">
         <v>-2988273.483416259</v>
       </c>
     </row>
@@ -631,6 +693,9 @@
         <v>2019706</v>
       </c>
       <c r="C21">
+        <v>2592245.056053067</v>
+      </c>
+      <c r="D21">
         <v>-572539.0560530671</v>
       </c>
     </row>
@@ -644,6 +709,9 @@
         <v>11608080</v>
       </c>
       <c r="C22">
+        <v>12764283.96898839</v>
+      </c>
+      <c r="D22">
         <v>-1156203.968988394</v>
       </c>
     </row>
@@ -657,6 +725,9 @@
         <v>3845083</v>
       </c>
       <c r="C23">
+        <v>18949844.13076285</v>
+      </c>
+      <c r="D23">
         <v>-15104761.13076285</v>
       </c>
     </row>
@@ -670,6 +741,9 @@
         <v>2019706</v>
       </c>
       <c r="C24">
+        <v>2238473.158789386</v>
+      </c>
+      <c r="D24">
         <v>-218767.1587893856</v>
       </c>
     </row>
@@ -683,6 +757,9 @@
         <v>17000000</v>
       </c>
       <c r="C25">
+        <v>14203975.93291875</v>
+      </c>
+      <c r="D25">
         <v>2796024.067081254</v>
       </c>
     </row>
@@ -696,6 +773,9 @@
         <v>8008680</v>
       </c>
       <c r="C26">
+        <v>12770549.65854063</v>
+      </c>
+      <c r="D26">
         <v>-4761869.658540631</v>
       </c>
     </row>
@@ -709,6 +789,9 @@
         <v>23883929</v>
       </c>
       <c r="C27">
+        <v>18774450.1393864</v>
+      </c>
+      <c r="D27">
         <v>5109478.860613603</v>
       </c>
     </row>
@@ -722,6 +805,9 @@
         <v>2600000</v>
       </c>
       <c r="C28">
+        <v>4352024.693781096</v>
+      </c>
+      <c r="D28">
         <v>-1752024.693781096</v>
       </c>
     </row>
@@ -735,6 +821,9 @@
         <v>2346614</v>
       </c>
       <c r="C29">
+        <v>5213215.098092868</v>
+      </c>
+      <c r="D29">
         <v>-2866601.098092868</v>
       </c>
     </row>
@@ -748,6 +837,9 @@
         <v>11710818</v>
       </c>
       <c r="C30">
+        <v>9522527.276782749</v>
+      </c>
+      <c r="D30">
         <v>2188290.723217251</v>
       </c>
     </row>
@@ -761,6 +853,9 @@
         <v>46741590</v>
       </c>
       <c r="C31">
+        <v>33393969.46616915</v>
+      </c>
+      <c r="D31">
         <v>13347620.53383085</v>
       </c>
     </row>
@@ -774,6 +869,9 @@
         <v>2019706</v>
       </c>
       <c r="C32">
+        <v>7106637.991625208</v>
+      </c>
+      <c r="D32">
         <v>-5086931.991625208</v>
       </c>
     </row>
@@ -787,6 +885,9 @@
         <v>2609400</v>
       </c>
       <c r="C33">
+        <v>3451816.070066334</v>
+      </c>
+      <c r="D33">
         <v>-842416.0700663342</v>
       </c>
     </row>
@@ -800,6 +901,9 @@
         <v>17000000</v>
       </c>
       <c r="C34">
+        <v>11404732.56890547</v>
+      </c>
+      <c r="D34">
         <v>5595267.431094525</v>
       </c>
     </row>
@@ -813,6 +917,9 @@
         <v>2019706</v>
       </c>
       <c r="C35">
+        <v>4970283.560613598</v>
+      </c>
+      <c r="D35">
         <v>-2950577.560613598</v>
       </c>
     </row>
@@ -826,6 +933,9 @@
         <v>4556983</v>
       </c>
       <c r="C36">
+        <v>8751431.871227197</v>
+      </c>
+      <c r="D36">
         <v>-4194448.871227197</v>
       </c>
     </row>
@@ -839,6 +949,9 @@
         <v>2066585</v>
       </c>
       <c r="C37">
+        <v>3615345.372885573</v>
+      </c>
+      <c r="D37">
         <v>-1548760.372885573</v>
       </c>
     </row>
@@ -852,6 +965,9 @@
         <v>5000000</v>
       </c>
       <c r="C38">
+        <v>8351812.898756221</v>
+      </c>
+      <c r="D38">
         <v>-3351812.898756221</v>
       </c>
     </row>
@@ -865,6 +981,9 @@
         <v>7245480</v>
       </c>
       <c r="C39">
+        <v>4519646.982504146</v>
+      </c>
+      <c r="D39">
         <v>2725833.017495854</v>
       </c>
     </row>
@@ -878,6 +997,9 @@
         <v>18700000</v>
       </c>
       <c r="C40">
+        <v>19988404.14875622</v>
+      </c>
+      <c r="D40">
         <v>-1288404.148756217</v>
       </c>
     </row>
@@ -891,6 +1013,9 @@
         <v>20000000</v>
       </c>
       <c r="C41">
+        <v>21586046.49535655</v>
+      </c>
+      <c r="D41">
         <v>-1586046.495356549</v>
       </c>
     </row>
@@ -904,6 +1029,9 @@
         <v>2019706</v>
       </c>
       <c r="C42">
+        <v>1969862.357131012</v>
+      </c>
+      <c r="D42">
         <v>49843.64286898798</v>
       </c>
     </row>
@@ -917,6 +1045,9 @@
         <v>36016200</v>
       </c>
       <c r="C43">
+        <v>34067399.70389718</v>
+      </c>
+      <c r="D43">
         <v>1948800.296102822</v>
       </c>
     </row>
@@ -930,6 +1061,9 @@
         <v>1836096</v>
       </c>
       <c r="C44">
+        <v>2594676.119237147</v>
+      </c>
+      <c r="D44">
         <v>-758580.1192371473</v>
       </c>
     </row>
@@ -943,6 +1077,9 @@
         <v>11750000</v>
       </c>
       <c r="C45">
+        <v>9552966.428855719</v>
+      </c>
+      <c r="D45">
         <v>2197033.571144281</v>
       </c>
     </row>
@@ -956,6 +1093,9 @@
         <v>4570080</v>
       </c>
       <c r="C46">
+        <v>3861766.214013267</v>
+      </c>
+      <c r="D46">
         <v>708313.7859867327</v>
       </c>
     </row>
@@ -969,6 +1109,9 @@
         <v>3071880</v>
       </c>
       <c r="C47">
+        <v>4385020.288308457</v>
+      </c>
+      <c r="D47">
         <v>-1313140.288308457</v>
       </c>
     </row>
@@ -982,6 +1125,9 @@
         <v>2949120</v>
       </c>
       <c r="C48">
+        <v>3492730.991210615</v>
+      </c>
+      <c r="D48">
         <v>-543610.9912106148</v>
       </c>
     </row>
@@ -995,6 +1141,9 @@
         <v>21700000</v>
       </c>
       <c r="C49">
+        <v>26988240.72363184</v>
+      </c>
+      <c r="D49">
         <v>-5288240.72363184</v>
       </c>
     </row>
@@ -1008,6 +1157,9 @@
         <v>7921300</v>
       </c>
       <c r="C50">
+        <v>16493797.06119403</v>
+      </c>
+      <c r="D50">
         <v>-8572497.061194031</v>
       </c>
     </row>
@@ -1021,6 +1173,9 @@
         <v>2165000</v>
       </c>
       <c r="C51">
+        <v>2632103.981923714</v>
+      </c>
+      <c r="D51">
         <v>-467103.9819237143</v>
       </c>
     </row>
@@ -1034,6 +1189,9 @@
         <v>22500000</v>
       </c>
       <c r="C52">
+        <v>22665456.91177447</v>
+      </c>
+      <c r="D52">
         <v>-165456.9117744677</v>
       </c>
     </row>
@@ -1047,6 +1205,9 @@
         <v>22627671</v>
       </c>
       <c r="C53">
+        <v>17714345.70124378</v>
+      </c>
+      <c r="D53">
         <v>4913325.298756219</v>
       </c>
     </row>
@@ -1060,6 +1221,9 @@
         <v>22000000</v>
       </c>
       <c r="C54">
+        <v>12770855.47636816</v>
+      </c>
+      <c r="D54">
         <v>9229144.523631843</v>
       </c>
     </row>
@@ -1073,6 +1237,9 @@
         <v>31830357</v>
       </c>
       <c r="C55">
+        <v>30021134.50887231</v>
+      </c>
+      <c r="D55">
         <v>1809222.491127688</v>
       </c>
     </row>
@@ -1086,6 +1253,9 @@
         <v>2413320</v>
       </c>
       <c r="C56">
+        <v>2847124.297097844</v>
+      </c>
+      <c r="D56">
         <v>-433804.2970978436</v>
       </c>
     </row>
@@ -1099,6 +1269,9 @@
         <v>2019706</v>
       </c>
       <c r="C57">
+        <v>4499338.606301823</v>
+      </c>
+      <c r="D57">
         <v>-2479632.606301823</v>
       </c>
     </row>
@@ -1112,6 +1285,9 @@
         <v>4000000</v>
       </c>
       <c r="C58">
+        <v>3192645.728192372</v>
+      </c>
+      <c r="D58">
         <v>807354.2718076278</v>
       </c>
     </row>
@@ -1125,6 +1301,9 @@
         <v>26346666</v>
       </c>
       <c r="C59">
+        <v>28581368.21069651</v>
+      </c>
+      <c r="D59">
         <v>-2234702.210696515</v>
       </c>
     </row>
@@ -1138,6 +1317,9 @@
         <v>2528233</v>
       </c>
       <c r="C60">
+        <v>3199122.685820896</v>
+      </c>
+      <c r="D60">
         <v>-670889.6858208957</v>
       </c>
     </row>
@@ -1151,6 +1333,9 @@
         <v>4094280</v>
       </c>
       <c r="C61">
+        <v>2955124.839220564</v>
+      </c>
+      <c r="D61">
         <v>1139155.160779436</v>
       </c>
     </row>
@@ -1164,6 +1349,9 @@
         <v>13033786</v>
       </c>
       <c r="C62">
+        <v>9727064.964096187</v>
+      </c>
+      <c r="D62">
         <v>3306721.035903813</v>
       </c>
     </row>
@@ -1177,6 +1365,9 @@
         <v>10489600</v>
       </c>
       <c r="C63">
+        <v>10457568.17935323</v>
+      </c>
+      <c r="D63">
         <v>32031.82064676844</v>
       </c>
     </row>
@@ -1190,6 +1381,9 @@
         <v>45183960</v>
       </c>
       <c r="C64">
+        <v>39779277.61973467</v>
+      </c>
+      <c r="D64">
         <v>5404682.380265325</v>
       </c>
     </row>
@@ -1203,6 +1397,9 @@
         <v>14704938</v>
       </c>
       <c r="C65">
+        <v>12221810.35257048</v>
+      </c>
+      <c r="D65">
         <v>2483127.647429518</v>
       </c>
     </row>
@@ -1216,6 +1413,9 @@
         <v>1119563</v>
       </c>
       <c r="C66">
+        <v>3426784.338225538</v>
+      </c>
+      <c r="D66">
         <v>-2307221.338225538</v>
       </c>
     </row>
@@ -1229,6 +1429,9 @@
         <v>20616000</v>
       </c>
       <c r="C67">
+        <v>16268427.26185738</v>
+      </c>
+      <c r="D67">
         <v>4347572.738142623</v>
       </c>
     </row>
@@ -1242,6 +1445,9 @@
         <v>6190476</v>
       </c>
       <c r="C68">
+        <v>6678704.586401328</v>
+      </c>
+      <c r="D68">
         <v>-488228.5864013284</v>
       </c>
     </row>
@@ -1255,6 +1461,9 @@
         <v>13050000</v>
       </c>
       <c r="C69">
+        <v>9861364.261857377</v>
+      </c>
+      <c r="D69">
         <v>3188635.738142623</v>
       </c>
     </row>
@@ -1268,6 +1477,9 @@
         <v>9460000</v>
       </c>
       <c r="C70">
+        <v>8962977.649087893</v>
+      </c>
+      <c r="D70">
         <v>497022.3509121072</v>
       </c>
     </row>
@@ -1281,6 +1493,9 @@
         <v>3000000</v>
       </c>
       <c r="C71">
+        <v>3810858.098424545</v>
+      </c>
+      <c r="D71">
         <v>-810858.0984245446</v>
       </c>
     </row>
@@ -1294,6 +1509,9 @@
         <v>1719864</v>
       </c>
       <c r="C72">
+        <v>2726357.195605306</v>
+      </c>
+      <c r="D72">
         <v>-1006493.195605306</v>
       </c>
     </row>
@@ -1307,6 +1525,9 @@
         <v>1119563</v>
       </c>
       <c r="C73">
+        <v>2495990.912686567</v>
+      </c>
+      <c r="D73">
         <v>-1376427.912686567</v>
       </c>
     </row>
@@ -1320,6 +1541,9 @@
         <v>23487629</v>
       </c>
       <c r="C74">
+        <v>23573854.34776122</v>
+      </c>
+      <c r="D74">
         <v>-86225.3477612175</v>
       </c>
     </row>
@@ -1333,6 +1557,9 @@
         <v>9625000</v>
       </c>
       <c r="C75">
+        <v>9790947.586815918</v>
+      </c>
+      <c r="D75">
         <v>-165947.5868159179</v>
       </c>
     </row>
@@ -1346,6 +1573,9 @@
         <v>3089520</v>
       </c>
       <c r="C76">
+        <v>3093984.922305142</v>
+      </c>
+      <c r="D76">
         <v>-4464.922305141576</v>
       </c>
     </row>
@@ -1359,6 +1589,9 @@
         <v>3666667</v>
       </c>
       <c r="C77">
+        <v>3918191.855306798</v>
+      </c>
+      <c r="D77">
         <v>-251524.8553067981</v>
       </c>
     </row>
@@ -1372,6 +1605,9 @@
         <v>25340000</v>
       </c>
       <c r="C78">
+        <v>21941769.01948591</v>
+      </c>
+      <c r="D78">
         <v>3398230.980514094</v>
       </c>
     </row>
@@ -1385,6 +1621,9 @@
         <v>7700000</v>
       </c>
       <c r="C79">
+        <v>9997366.924378112</v>
+      </c>
+      <c r="D79">
         <v>-2297366.924378112</v>
       </c>
     </row>
@@ -1398,6 +1637,9 @@
         <v>24360000</v>
       </c>
       <c r="C80">
+        <v>22359066.70713101</v>
+      </c>
+      <c r="D80">
         <v>2000933.292868994</v>
       </c>
     </row>
@@ -1411,6 +1653,9 @@
         <v>9423869</v>
       </c>
       <c r="C81">
+        <v>7766830.153731346</v>
+      </c>
+      <c r="D81">
         <v>1657038.846268654</v>
       </c>
     </row>
@@ -1424,6 +1669,9 @@
         <v>6614280</v>
       </c>
       <c r="C82">
+        <v>6729383.969485906</v>
+      </c>
+      <c r="D82">
         <v>-115103.969485906</v>
       </c>
     </row>
@@ -1437,6 +1685,9 @@
         <v>11692308</v>
       </c>
       <c r="C83">
+        <v>9373159.169154225</v>
+      </c>
+      <c r="D83">
         <v>2319148.830845775</v>
       </c>
     </row>
@@ -1450,6 +1701,9 @@
         <v>2528233</v>
       </c>
       <c r="C84">
+        <v>5444019.728358208</v>
+      </c>
+      <c r="D84">
         <v>-2915786.728358208</v>
       </c>
     </row>
@@ -1463,6 +1717,9 @@
         <v>2019706</v>
       </c>
       <c r="C85">
+        <v>5580379.43026534</v>
+      </c>
+      <c r="D85">
         <v>-3560673.43026534</v>
       </c>
     </row>
@@ -1476,6 +1733,9 @@
         <v>11055360</v>
       </c>
       <c r="C86">
+        <v>13196600.52064677</v>
+      </c>
+      <c r="D86">
         <v>-2141240.52064677</v>
       </c>
     </row>
@@ -1489,6 +1749,9 @@
         <v>4000000</v>
       </c>
       <c r="C87">
+        <v>7864160.211276948</v>
+      </c>
+      <c r="D87">
         <v>-3864160.211276948</v>
       </c>
     </row>
@@ -1502,6 +1765,9 @@
         <v>51915615</v>
       </c>
       <c r="C88">
+        <v>43399545.18192374</v>
+      </c>
+      <c r="D88">
         <v>8516069.81807626</v>
       </c>
     </row>
@@ -1515,6 +1781,9 @@
         <v>5784120</v>
       </c>
       <c r="C89">
+        <v>4839207.802321726</v>
+      </c>
+      <c r="D89">
         <v>944912.1976782745</v>
       </c>
     </row>
@@ -1528,6 +1797,9 @@
         <v>40600080</v>
       </c>
       <c r="C90">
+        <v>37477788.58532339</v>
+      </c>
+      <c r="D90">
         <v>3122291.414676607</v>
       </c>
     </row>
@@ -1541,6 +1813,9 @@
         <v>5050800</v>
       </c>
       <c r="C91">
+        <v>3413814.039220563</v>
+      </c>
+      <c r="D91">
         <v>1636985.960779437</v>
       </c>
     </row>
@@ -1554,6 +1829,9 @@
         <v>28600000</v>
       </c>
       <c r="C92">
+        <v>29939983.15472636</v>
+      </c>
+      <c r="D92">
         <v>-1339983.154726364</v>
       </c>
     </row>
@@ -1567,6 +1845,9 @@
         <v>4536720</v>
       </c>
       <c r="C93">
+        <v>3814132.757296849</v>
+      </c>
+      <c r="D93">
         <v>722587.242703151</v>
       </c>
     </row>
@@ -1580,6 +1861,9 @@
         <v>4798440</v>
       </c>
       <c r="C94">
+        <v>3941958.277777778</v>
+      </c>
+      <c r="D94">
         <v>856481.7222222215</v>
       </c>
     </row>
@@ -1593,6 +1877,9 @@
         <v>20357143</v>
       </c>
       <c r="C95">
+        <v>22577366.41849088</v>
+      </c>
+      <c r="D95">
         <v>-2220223.418490879</v>
       </c>
     </row>
@@ -1606,6 +1893,9 @@
         <v>10900000</v>
       </c>
       <c r="C96">
+        <v>6071642.013847428</v>
+      </c>
+      <c r="D96">
         <v>4828357.986152572</v>
       </c>
     </row>
@@ -1619,6 +1909,9 @@
         <v>40064220</v>
       </c>
       <c r="C97">
+        <v>37208486.67255389</v>
+      </c>
+      <c r="D97">
         <v>2855733.327446111</v>
       </c>
     </row>
@@ -1632,6 +1925,9 @@
         <v>15277778</v>
       </c>
       <c r="C98">
+        <v>8190127.901907135</v>
+      </c>
+      <c r="D98">
         <v>7087650.098092865</v>
       </c>
     </row>
@@ -1645,6 +1941,9 @@
         <v>6481482</v>
       </c>
       <c r="C99">
+        <v>3950105.943034827</v>
+      </c>
+      <c r="D99">
         <v>2531376.056965173</v>
       </c>
     </row>
@@ -1658,6 +1957,9 @@
         <v>3360000</v>
       </c>
       <c r="C100">
+        <v>7424288.259701491</v>
+      </c>
+      <c r="D100">
         <v>-4064288.259701491</v>
       </c>
     </row>
@@ -1671,6 +1973,9 @@
         <v>4124400</v>
       </c>
       <c r="C101">
+        <v>3747657.79676617</v>
+      </c>
+      <c r="D101">
         <v>376742.2032338302</v>
       </c>
     </row>
@@ -1684,6 +1989,9 @@
         <v>2586665</v>
       </c>
       <c r="C102">
+        <v>7068409.540215587</v>
+      </c>
+      <c r="D102">
         <v>-4481744.540215587</v>
       </c>
     </row>
@@ -1697,6 +2005,9 @@
         <v>47649433</v>
       </c>
       <c r="C103">
+        <v>39880084.903068</v>
+      </c>
+      <c r="D103">
         <v>7769348.096932001</v>
       </c>
     </row>
@@ -1710,6 +2021,9 @@
         <v>4330680</v>
       </c>
       <c r="C104">
+        <v>8125976.704477613</v>
+      </c>
+      <c r="D104">
         <v>-3795296.704477613</v>
       </c>
     </row>
@@ -1723,6 +2037,9 @@
         <v>3527160</v>
       </c>
       <c r="C105">
+        <v>4718281.38432836</v>
+      </c>
+      <c r="D105">
         <v>-1191121.38432836</v>
       </c>
     </row>
@@ -1736,6 +2053,9 @@
         <v>13534817</v>
       </c>
       <c r="C106">
+        <v>16017361.50298508</v>
+      </c>
+      <c r="D106">
         <v>-2482544.502985081</v>
       </c>
     </row>
@@ -1749,6 +2069,9 @@
         <v>1927896</v>
       </c>
       <c r="C107">
+        <v>1915928.677611941</v>
+      </c>
+      <c r="D107">
         <v>11967.32238805923</v>
       </c>
     </row>
@@ -1762,6 +2085,9 @@
         <v>47607350</v>
       </c>
       <c r="C108">
+        <v>40366560.94046434</v>
+      </c>
+      <c r="D108">
         <v>7240789.05953566</v>
       </c>
     </row>
@@ -1775,6 +2101,9 @@
         <v>2346614</v>
       </c>
       <c r="C109">
+        <v>2984881.471227199</v>
+      </c>
+      <c r="D109">
         <v>-638267.4712271988</v>
       </c>
     </row>
@@ -1788,6 +2117,9 @@
         <v>3000000</v>
       </c>
       <c r="C110">
+        <v>4495568.202736318</v>
+      </c>
+      <c r="D110">
         <v>-1495568.202736318</v>
       </c>
     </row>
@@ -1801,6 +2133,9 @@
         <v>2581522</v>
       </c>
       <c r="C111">
+        <v>2643965.3907131</v>
+      </c>
+      <c r="D111">
         <v>-62443.39071310032</v>
       </c>
     </row>
@@ -1814,6 +2149,9 @@
         <v>13932008</v>
       </c>
       <c r="C112">
+        <v>12354557.55638475</v>
+      </c>
+      <c r="D112">
         <v>1577450.443615254</v>
       </c>
     </row>
@@ -1827,6 +2165,9 @@
         <v>3873025</v>
       </c>
       <c r="C113">
+        <v>4058848.504145937</v>
+      </c>
+      <c r="D113">
         <v>-185823.504145937</v>
       </c>
     </row>
@@ -1840,6 +2181,9 @@
         <v>3044872</v>
       </c>
       <c r="C114">
+        <v>4302587.502155887</v>
+      </c>
+      <c r="D114">
         <v>-1257715.502155887</v>
       </c>
     </row>
@@ -1853,6 +2197,9 @@
         <v>18857143</v>
       </c>
       <c r="C115">
+        <v>13146823.93457712</v>
+      </c>
+      <c r="D115">
         <v>5710319.065422883</v>
       </c>
     </row>
@@ -1866,6 +2213,9 @@
         <v>32600060</v>
       </c>
       <c r="C116">
+        <v>31540049.54991708</v>
+      </c>
+      <c r="D116">
         <v>1060010.45008292</v>
       </c>
     </row>
@@ -1879,6 +2229,9 @@
         <v>17000000</v>
       </c>
       <c r="C117">
+        <v>14449427.14386401</v>
+      </c>
+      <c r="D117">
         <v>2550572.85613599</v>
       </c>
     </row>
@@ -1892,6 +2245,9 @@
         <v>12402000</v>
       </c>
       <c r="C118">
+        <v>8582370.764510781</v>
+      </c>
+      <c r="D118">
         <v>3819629.235489219</v>
       </c>
     </row>
@@ -1905,6 +2261,9 @@
         <v>6802950</v>
       </c>
       <c r="C119">
+        <v>7217136.857131009</v>
+      </c>
+      <c r="D119">
         <v>-414186.857131009</v>
       </c>
     </row>
@@ -1918,6 +2277,9 @@
         <v>34005250</v>
       </c>
       <c r="C120">
+        <v>29943634.10771145</v>
+      </c>
+      <c r="D120">
         <v>4061615.892288554</v>
       </c>
     </row>
@@ -1931,6 +2293,9 @@
         <v>3889800</v>
       </c>
       <c r="C121">
+        <v>6669316.265505807</v>
+      </c>
+      <c r="D121">
         <v>-2779516.265505807</v>
       </c>
     </row>
@@ -1944,6 +2309,9 @@
         <v>45640084</v>
       </c>
       <c r="C122">
+        <v>40451358.87189057</v>
+      </c>
+      <c r="D122">
         <v>5188725.128109433</v>
       </c>
     </row>
@@ -1957,6 +2325,9 @@
         <v>6587040</v>
       </c>
       <c r="C123">
+        <v>9109246.218988394</v>
+      </c>
+      <c r="D123">
         <v>-2522206.218988394</v>
       </c>
     </row>
@@ -1970,6 +2341,9 @@
         <v>2019706</v>
       </c>
       <c r="C124">
+        <v>2330333.857545604</v>
+      </c>
+      <c r="D124">
         <v>-310627.8575456045</v>
       </c>
     </row>
@@ -1983,6 +2357,9 @@
         <v>33386850</v>
       </c>
       <c r="C125">
+        <v>32447062.71475954</v>
+      </c>
+      <c r="D125">
         <v>939787.2852404639</v>
       </c>
     </row>
@@ -1996,6 +2373,9 @@
         <v>1997238</v>
       </c>
       <c r="C126">
+        <v>3734149.63747927</v>
+      </c>
+      <c r="D126">
         <v>-1736911.63747927</v>
       </c>
     </row>
@@ -2009,6 +2389,9 @@
         <v>41000000</v>
       </c>
       <c r="C127">
+        <v>21063866.05074627</v>
+      </c>
+      <c r="D127">
         <v>19936133.94925373</v>
       </c>
     </row>
@@ -2022,6 +2405,9 @@
         <v>1927896</v>
       </c>
       <c r="C128">
+        <v>2674418.34145937</v>
+      </c>
+      <c r="D128">
         <v>-746522.3414593698</v>
       </c>
     </row>
@@ -2035,6 +2421,9 @@
         <v>22266182</v>
       </c>
       <c r="C129">
+        <v>20838735.2946932</v>
+      </c>
+      <c r="D129">
         <v>1427446.705306798</v>
       </c>
     </row>
@@ -2048,6 +2437,9 @@
         <v>3196448</v>
       </c>
       <c r="C130">
+        <v>10269679.93524047</v>
+      </c>
+      <c r="D130">
         <v>-7073231.935240466</v>
       </c>
     </row>
@@ -2061,6 +2453,9 @@
         <v>12100000</v>
       </c>
       <c r="C131">
+        <v>8867658.796766171</v>
+      </c>
+      <c r="D131">
         <v>3232341.203233829</v>
       </c>
     </row>
@@ -2074,6 +2469,9 @@
         <v>27586207</v>
       </c>
       <c r="C132">
+        <v>25740458.2136816</v>
+      </c>
+      <c r="D132">
         <v>1845748.786318399</v>
       </c>
     </row>
@@ -2087,6 +2485,9 @@
         <v>1901769</v>
       </c>
       <c r="C133">
+        <v>2425578.564925373</v>
+      </c>
+      <c r="D133">
         <v>-523809.5649253731</v>
       </c>
     </row>
@@ -2100,6 +2501,9 @@
         <v>200000</v>
       </c>
       <c r="C134">
+        <v>2765488.212769486</v>
+      </c>
+      <c r="D134">
         <v>-2565488.212769486</v>
       </c>
     </row>
@@ -2113,6 +2517,9 @@
         <v>22321429</v>
       </c>
       <c r="C135">
+        <v>18141023.50008292</v>
+      </c>
+      <c r="D135">
         <v>4180405.499917079</v>
       </c>
     </row>
@@ -2126,6 +2533,9 @@
         <v>9891480</v>
       </c>
       <c r="C136">
+        <v>10253953.08134329</v>
+      </c>
+      <c r="D136">
         <v>-362473.0813432857</v>
       </c>
     </row>
@@ -2139,6 +2549,9 @@
         <v>9600000</v>
       </c>
       <c r="C137">
+        <v>9712566.11849088</v>
+      </c>
+      <c r="D137">
         <v>-112566.1184908804</v>
       </c>
     </row>
@@ -2152,6 +2565,9 @@
         <v>4765339</v>
       </c>
       <c r="C138">
+        <v>5013981.34154229</v>
+      </c>
+      <c r="D138">
         <v>-248642.3415422896</v>
       </c>
     </row>
@@ -2165,6 +2581,9 @@
         <v>3712920</v>
       </c>
       <c r="C139">
+        <v>3604775.638391376</v>
+      </c>
+      <c r="D139">
         <v>108144.361608624</v>
       </c>
     </row>
@@ -2178,6 +2597,9 @@
         <v>2385720</v>
       </c>
       <c r="C140">
+        <v>3249520.99668325</v>
+      </c>
+      <c r="D140">
         <v>-863800.9966832502</v>
       </c>
     </row>
@@ -2191,6 +2613,9 @@
         <v>1119563</v>
       </c>
       <c r="C141">
+        <v>1943438.953150913</v>
+      </c>
+      <c r="D141">
         <v>-823875.9531509127</v>
       </c>
     </row>
@@ -2204,6 +2629,9 @@
         <v>15740741</v>
       </c>
       <c r="C142">
+        <v>11152920.12089552</v>
+      </c>
+      <c r="D142">
         <v>4587820.879104478</v>
       </c>
     </row>
@@ -2217,6 +2645,9 @@
         <v>5808435</v>
       </c>
       <c r="C143">
+        <v>20435703.4973466</v>
+      </c>
+      <c r="D143">
         <v>-14627268.4973466</v>
       </c>
     </row>
@@ -2230,6 +2661,9 @@
         <v>17897728</v>
       </c>
       <c r="C144">
+        <v>20042649.61028193</v>
+      </c>
+      <c r="D144">
         <v>-2144921.610281926</v>
       </c>
     </row>
@@ -2243,6 +2677,9 @@
         <v>35640000</v>
       </c>
       <c r="C145">
+        <v>35113727.77529021</v>
+      </c>
+      <c r="D145">
         <v>526272.2247097939</v>
       </c>
     </row>
@@ -2256,6 +2693,9 @@
         <v>1719864</v>
       </c>
       <c r="C146">
+        <v>4011360.934411278</v>
+      </c>
+      <c r="D146">
         <v>-2291496.934411278</v>
       </c>
     </row>
@@ -2269,6 +2709,9 @@
         <v>13000000</v>
       </c>
       <c r="C147">
+        <v>7336183.673217244</v>
+      </c>
+      <c r="D147">
         <v>5663816.326782756</v>
       </c>
     </row>
@@ -2282,6 +2725,9 @@
         <v>19928571</v>
       </c>
       <c r="C148">
+        <v>14776457.62131011</v>
+      </c>
+      <c r="D148">
         <v>5152113.378689885</v>
       </c>
     </row>
@@ -2295,6 +2741,9 @@
         <v>39270150</v>
       </c>
       <c r="C149">
+        <v>26828752.68101161</v>
+      </c>
+      <c r="D149">
         <v>12441397.31898839</v>
       </c>
     </row>
@@ -2308,6 +2757,9 @@
         <v>12960000</v>
       </c>
       <c r="C150">
+        <v>12089566.51824212</v>
+      </c>
+      <c r="D150">
         <v>870433.4817578811</v>
       </c>
     </row>
@@ -2321,6 +2773,9 @@
         <v>9245121</v>
       </c>
       <c r="C151">
+        <v>4907492.879601992</v>
+      </c>
+      <c r="D151">
         <v>4337628.120398008</v>
       </c>
     </row>
@@ -2334,6 +2789,9 @@
         <v>1927896</v>
       </c>
       <c r="C152">
+        <v>3642021.298590383</v>
+      </c>
+      <c r="D152">
         <v>-1714125.298590383</v>
       </c>
     </row>
@@ -2347,6 +2805,9 @@
         <v>4310160</v>
       </c>
       <c r="C153">
+        <v>5033729.485074627</v>
+      </c>
+      <c r="D153">
         <v>-723569.4850746272</v>
       </c>
     </row>
@@ -2360,6 +2821,9 @@
         <v>2165000</v>
       </c>
       <c r="C154">
+        <v>2501374.757379767</v>
+      </c>
+      <c r="D154">
         <v>-336374.7573797675</v>
       </c>
     </row>
@@ -2373,6 +2837,9 @@
         <v>7413955</v>
       </c>
       <c r="C155">
+        <v>7556655.58698176</v>
+      </c>
+      <c r="D155">
         <v>-142700.5869817603</v>
       </c>
     </row>
@@ -2386,6 +2853,9 @@
         <v>31500000</v>
       </c>
       <c r="C156">
+        <v>26398199.26285241</v>
+      </c>
+      <c r="D156">
         <v>5101800.737147592</v>
       </c>
     </row>
@@ -2399,6 +2869,9 @@
         <v>9770880</v>
       </c>
       <c r="C157">
+        <v>10794615.61202322</v>
+      </c>
+      <c r="D157">
         <v>-1023735.612023218</v>
       </c>
     </row>
@@ -2412,6 +2885,9 @@
         <v>5569920</v>
       </c>
       <c r="C158">
+        <v>4697865.791873964</v>
+      </c>
+      <c r="D158">
         <v>872054.2081260365</v>
       </c>
     </row>
@@ -2425,6 +2901,9 @@
         <v>27000000</v>
       </c>
       <c r="C159">
+        <v>27429952.25978441</v>
+      </c>
+      <c r="D159">
         <v>-429952.2597844079</v>
       </c>
     </row>
@@ -2438,6 +2917,9 @@
         <v>19279841</v>
       </c>
       <c r="C160">
+        <v>16642648.1221393</v>
+      </c>
+      <c r="D160">
         <v>2637192.877860704</v>
       </c>
     </row>
@@ -2451,6 +2933,9 @@
         <v>1902137</v>
       </c>
       <c r="C161">
+        <v>5315233.163515755</v>
+      </c>
+      <c r="D161">
         <v>-3413096.163515755</v>
       </c>
     </row>
@@ -2464,6 +2949,9 @@
         <v>2019706</v>
       </c>
       <c r="C162">
+        <v>3704183.609203981</v>
+      </c>
+      <c r="D162">
         <v>-1684477.609203981</v>
       </c>
     </row>
@@ -2477,6 +2965,9 @@
         <v>36861707</v>
       </c>
       <c r="C163">
+        <v>25678055.9623549</v>
+      </c>
+      <c r="D163">
         <v>11183651.0376451</v>
       </c>
     </row>
@@ -2490,6 +2981,9 @@
         <v>2019706</v>
       </c>
       <c r="C164">
+        <v>9577118.626533996</v>
+      </c>
+      <c r="D164">
         <v>-7557412.626533996</v>
       </c>
     </row>
@@ -2503,6 +2997,9 @@
         <v>12046020</v>
       </c>
       <c r="C165">
+        <v>5479820.213847429</v>
+      </c>
+      <c r="D165">
         <v>6566199.786152571</v>
       </c>
     </row>
@@ -2516,6 +3013,9 @@
         <v>10386000</v>
       </c>
       <c r="C166">
+        <v>9957705.292039802</v>
+      </c>
+      <c r="D166">
         <v>428294.7079601977</v>
       </c>
     </row>
@@ -2529,6 +3029,9 @@
         <v>3695040</v>
       </c>
       <c r="C167">
+        <v>3610869.158789386</v>
+      </c>
+      <c r="D167">
         <v>84170.84121061396</v>
       </c>
     </row>
@@ -2542,6 +3045,9 @@
         <v>10000000</v>
       </c>
       <c r="C168">
+        <v>10090199.68913764</v>
+      </c>
+      <c r="D168">
         <v>-90199.6891376432</v>
       </c>
     </row>
@@ -2555,6 +3061,9 @@
         <v>11020000</v>
       </c>
       <c r="C169">
+        <v>9324838.510447767</v>
+      </c>
+      <c r="D169">
         <v>1695161.489552233</v>
       </c>
     </row>
@@ -2568,6 +3077,9 @@
         <v>4310250</v>
       </c>
       <c r="C170">
+        <v>5330811.186401328</v>
+      </c>
+      <c r="D170">
         <v>-1020561.186401328</v>
       </c>
     </row>
@@ -2581,6 +3093,9 @@
         <v>2000000</v>
       </c>
       <c r="C171">
+        <v>2600286.236567164</v>
+      </c>
+      <c r="D171">
         <v>-600286.2365671638</v>
       </c>
     </row>
@@ -2594,6 +3109,9 @@
         <v>5026800</v>
       </c>
       <c r="C172">
+        <v>3333798.319402985</v>
+      </c>
+      <c r="D172">
         <v>1693001.680597015</v>
       </c>
     </row>
@@ -2607,6 +3125,9 @@
         <v>15669643</v>
       </c>
       <c r="C173">
+        <v>11763296.05762853</v>
+      </c>
+      <c r="D173">
         <v>3906346.942371475</v>
       </c>
     </row>
@@ -2620,6 +3141,9 @@
         <v>20089286</v>
       </c>
       <c r="C174">
+        <v>19544181.07172471</v>
+      </c>
+      <c r="D174">
         <v>545104.9282752872</v>
       </c>
     </row>
@@ -2633,6 +3157,9 @@
         <v>2306400</v>
       </c>
       <c r="C175">
+        <v>3428431.28955224</v>
+      </c>
+      <c r="D175">
         <v>-1122031.28955224</v>
       </c>
     </row>
@@ -2646,6 +3173,9 @@
         <v>11000000</v>
       </c>
       <c r="C176">
+        <v>7352295.360862354</v>
+      </c>
+      <c r="D176">
         <v>3647704.639137646</v>
       </c>
     </row>
@@ -2659,6 +3189,9 @@
         <v>33833400</v>
       </c>
       <c r="C177">
+        <v>31639623.26865673</v>
+      </c>
+      <c r="D177">
         <v>2193776.731343269</v>
       </c>
     </row>
@@ -2672,6 +3205,9 @@
         <v>37037037</v>
       </c>
       <c r="C178">
+        <v>30070868.0876451</v>
+      </c>
+      <c r="D178">
         <v>6966168.912354898</v>
       </c>
     </row>
@@ -2685,6 +3221,9 @@
         <v>17400000</v>
       </c>
       <c r="C179">
+        <v>5012723.075953563</v>
+      </c>
+      <c r="D179">
         <v>12387276.92404644</v>
       </c>
     </row>
@@ -2698,6 +3237,9 @@
         <v>7614480</v>
       </c>
       <c r="C180">
+        <v>8348209.859286899</v>
+      </c>
+      <c r="D180">
         <v>-733729.8592868987</v>
       </c>
     </row>
@@ -2711,6 +3253,9 @@
         <v>1119563</v>
       </c>
       <c r="C181">
+        <v>2037395.926699834</v>
+      </c>
+      <c r="D181">
         <v>-917832.9266998344</v>
       </c>
     </row>
@@ -2724,6 +3269,9 @@
         <v>2696280</v>
       </c>
       <c r="C182">
+        <v>3213533.521973467</v>
+      </c>
+      <c r="D182">
         <v>-517253.5219734665</v>
       </c>
     </row>
@@ -2737,6 +3285,9 @@
         <v>27102202</v>
       </c>
       <c r="C183">
+        <v>26777424.93134328</v>
+      </c>
+      <c r="D183">
         <v>324777.0686567165</v>
       </c>
     </row>
@@ -2750,6 +3301,9 @@
         <v>5000000</v>
       </c>
       <c r="C184">
+        <v>7224343.895688227</v>
+      </c>
+      <c r="D184">
         <v>-2224343.895688227</v>
       </c>
     </row>
@@ -2763,6 +3317,9 @@
         <v>1119563</v>
       </c>
       <c r="C185">
+        <v>2098981.832587066</v>
+      </c>
+      <c r="D185">
         <v>-979418.8325870656</v>
       </c>
     </row>
@@ -2776,6 +3333,9 @@
         <v>47607350</v>
       </c>
       <c r="C186">
+        <v>37312298.8818408</v>
+      </c>
+      <c r="D186">
         <v>10295051.1181592</v>
       </c>
     </row>
@@ -2789,6 +3349,9 @@
         <v>3510600</v>
       </c>
       <c r="C187">
+        <v>7370589.179767828</v>
+      </c>
+      <c r="D187">
         <v>-3859989.179767828</v>
       </c>
     </row>
@@ -2802,6 +3365,9 @@
         <v>2066585</v>
       </c>
       <c r="C188">
+        <v>2053420.675456054</v>
+      </c>
+      <c r="D188">
         <v>13164.32454394619</v>
       </c>
     </row>
@@ -2815,6 +3381,9 @@
         <v>2439025</v>
       </c>
       <c r="C189">
+        <v>3195714.840049752</v>
+      </c>
+      <c r="D189">
         <v>-756689.8400497516</v>
       </c>
     </row>
@@ -2828,6 +3397,9 @@
         <v>1997238</v>
       </c>
       <c r="C190">
+        <v>3422856.949751243</v>
+      </c>
+      <c r="D190">
         <v>-1425618.949751243</v>
       </c>
     </row>
@@ -2841,6 +3413,9 @@
         <v>25679348</v>
       </c>
       <c r="C191">
+        <v>20988810.12736318</v>
+      </c>
+      <c r="D191">
         <v>4690537.872636817</v>
       </c>
     </row>
@@ -2854,6 +3429,9 @@
         <v>2925360</v>
       </c>
       <c r="C192">
+        <v>7387684.720066336</v>
+      </c>
+      <c r="D192">
         <v>-4462324.720066336</v>
       </c>
     </row>
@@ -2867,6 +3445,9 @@
         <v>20000000</v>
       </c>
       <c r="C193">
+        <v>18797304.53988392</v>
+      </c>
+      <c r="D193">
         <v>1202695.460116085</v>
       </c>
     </row>
@@ -2880,6 +3461,9 @@
         <v>47607350</v>
       </c>
       <c r="C194">
+        <v>41581763.22819237</v>
+      </c>
+      <c r="D194">
         <v>6025586.771807633</v>
       </c>
     </row>
@@ -2893,6 +3477,9 @@
         <v>2019706</v>
       </c>
       <c r="C195">
+        <v>2070567.707877281</v>
+      </c>
+      <c r="D195">
         <v>-50861.70787728066</v>
       </c>
     </row>
@@ -2906,6 +3493,9 @@
         <v>2586665</v>
       </c>
       <c r="C196">
+        <v>2598277.646849088</v>
+      </c>
+      <c r="D196">
         <v>-11612.64684908791</v>
       </c>
     </row>
@@ -2919,6 +3509,9 @@
         <v>5379706</v>
       </c>
       <c r="C197">
+        <v>6498838.839220564</v>
+      </c>
+      <c r="D197">
         <v>-1119132.839220564</v>
       </c>
     </row>
@@ -2932,6 +3525,9 @@
         <v>12015150</v>
       </c>
       <c r="C198">
+        <v>10462085.38175787</v>
+      </c>
+      <c r="D198">
         <v>1553064.618242126</v>
       </c>
     </row>
@@ -2945,6 +3541,9 @@
         <v>9895833</v>
       </c>
       <c r="C199">
+        <v>9687335.258374793</v>
+      </c>
+      <c r="D199">
         <v>208497.7416252065</v>
       </c>
     </row>
@@ -2958,6 +3557,9 @@
         <v>14000000</v>
       </c>
       <c r="C200">
+        <v>14967186.94660033</v>
+      </c>
+      <c r="D200">
         <v>-967186.946600331</v>
       </c>
     </row>
@@ -2971,6 +3573,9 @@
         <v>2019706</v>
       </c>
       <c r="C201">
+        <v>6123935.955389718</v>
+      </c>
+      <c r="D201">
         <v>-4104229.955389718</v>
       </c>
     </row>
@@ -2984,6 +3589,9 @@
         <v>2019706</v>
       </c>
       <c r="C202">
+        <v>4143881.353067994</v>
+      </c>
+      <c r="D202">
         <v>-2124175.353067994</v>
       </c>
     </row>
@@ -2997,6 +3605,9 @@
         <v>2352000</v>
       </c>
       <c r="C203">
+        <v>3294690.055721394</v>
+      </c>
+      <c r="D203">
         <v>-942690.0557213943</v>
       </c>
     </row>
@@ -3010,6 +3621,9 @@
         <v>14763636</v>
       </c>
       <c r="C204">
+        <v>9579263.525953563</v>
+      </c>
+      <c r="D204">
         <v>5184372.474046437</v>
       </c>
     </row>
@@ -3023,6 +3637,9 @@
         <v>2831160</v>
       </c>
       <c r="C205">
+        <v>4418705.311359867</v>
+      </c>
+      <c r="D205">
         <v>-1587545.311359867</v>
       </c>
     </row>
@@ -3036,6 +3653,9 @@
         <v>3722040</v>
       </c>
       <c r="C206">
+        <v>4905337.901243782</v>
+      </c>
+      <c r="D206">
         <v>-1183297.901243782</v>
       </c>
     </row>
@@ -3049,6 +3669,9 @@
         <v>11000000</v>
       </c>
       <c r="C207">
+        <v>8564308.439303486</v>
+      </c>
+      <c r="D207">
         <v>2435691.560696514</v>
       </c>
     </row>
@@ -3062,6 +3685,9 @@
         <v>1845593</v>
       </c>
       <c r="C208">
+        <v>3909689.572470977</v>
+      </c>
+      <c r="D208">
         <v>-2064096.572470977</v>
       </c>
     </row>
@@ -3075,6 +3701,9 @@
         <v>2400000</v>
       </c>
       <c r="C209">
+        <v>3756256.886152571</v>
+      </c>
+      <c r="D209">
         <v>-1356256.886152571</v>
       </c>
     </row>
@@ -3088,6 +3717,9 @@
         <v>5370370</v>
       </c>
       <c r="C210">
+        <v>2159394.59013267</v>
+      </c>
+      <c r="D210">
         <v>3210975.40986733</v>
       </c>
     </row>
@@ -3101,6 +3733,9 @@
         <v>2413304</v>
       </c>
       <c r="C211">
+        <v>4187311.43482587</v>
+      </c>
+      <c r="D211">
         <v>-1774007.43482587</v>
       </c>
     </row>
@@ -3114,6 +3749,9 @@
         <v>6012840</v>
       </c>
       <c r="C212">
+        <v>5777911.063764513</v>
+      </c>
+      <c r="D212">
         <v>234928.9362354875</v>
       </c>
     </row>
@@ -3127,6 +3765,9 @@
         <v>25568182</v>
       </c>
       <c r="C213">
+        <v>27620960.17230514</v>
+      </c>
+      <c r="D213">
         <v>-2052778.172305141</v>
       </c>
     </row>
@@ -3140,6 +3781,9 @@
         <v>8000000</v>
       </c>
       <c r="C214">
+        <v>6932049.290132671</v>
+      </c>
+      <c r="D214">
         <v>1067950.709867329</v>
       </c>
     </row>
@@ -3153,6 +3797,9 @@
         <v>3199920</v>
       </c>
       <c r="C215">
+        <v>2961210.262603649</v>
+      </c>
+      <c r="D215">
         <v>238709.7373963506</v>
       </c>
     </row>
@@ -3166,6 +3813,9 @@
         <v>40064220</v>
       </c>
       <c r="C216">
+        <v>33759726.2309287</v>
+      </c>
+      <c r="D216">
         <v>6304493.769071303</v>
       </c>
     </row>
@@ -3179,6 +3829,9 @@
         <v>2019706</v>
       </c>
       <c r="C217">
+        <v>3051059.139883915</v>
+      </c>
+      <c r="D217">
         <v>-1031353.139883915</v>
       </c>
     </row>
@@ -3192,6 +3845,9 @@
         <v>45640084</v>
       </c>
       <c r="C218">
+        <v>39509759.61160863</v>
+      </c>
+      <c r="D218">
         <v>6130324.388391368</v>
       </c>
     </row>
@@ -3205,6 +3861,9 @@
         <v>15384616</v>
       </c>
       <c r="C219">
+        <v>19324268.03772803</v>
+      </c>
+      <c r="D219">
         <v>-3939652.03772803</v>
       </c>
     </row>
@@ -3218,6 +3877,9 @@
         <v>5722116</v>
       </c>
       <c r="C220">
+        <v>4834658.416749586</v>
+      </c>
+      <c r="D220">
         <v>887457.5832504136</v>
       </c>
     </row>
@@ -3231,6 +3893,9 @@
         <v>1119563</v>
       </c>
       <c r="C221">
+        <v>1516717.772968491</v>
+      </c>
+      <c r="D221">
         <v>-397154.7729684906</v>
       </c>
     </row>
@@ -3244,6 +3909,9 @@
         <v>1801769</v>
       </c>
       <c r="C222">
+        <v>1990781.23681592</v>
+      </c>
+      <c r="D222">
         <v>-189012.2368159203</v>
       </c>
     </row>
@@ -3257,6 +3925,9 @@
         <v>45640084</v>
       </c>
       <c r="C223">
+        <v>40550309.96351576</v>
+      </c>
+      <c r="D223">
         <v>5089774.036484241</v>
       </c>
     </row>
@@ -3270,6 +3941,9 @@
         <v>6250000</v>
       </c>
       <c r="C224">
+        <v>5103724.795854065</v>
+      </c>
+      <c r="D224">
         <v>1146275.204145935</v>
       </c>
     </row>
@@ -3283,6 +3957,9 @@
         <v>4775640</v>
       </c>
       <c r="C225">
+        <v>5067426.672222223</v>
+      </c>
+      <c r="D225">
         <v>-291786.6722222231</v>
       </c>
     </row>
@@ -3296,6 +3973,9 @@
         <v>1836096</v>
       </c>
       <c r="C226">
+        <v>6080386.498839137</v>
+      </c>
+      <c r="D226">
         <v>-4244290.498839137</v>
       </c>
     </row>
@@ -3309,6 +3989,9 @@
         <v>1119563</v>
       </c>
       <c r="C227">
+        <v>1677285.630845771</v>
+      </c>
+      <c r="D227">
         <v>-557722.6308457709</v>
       </c>
     </row>
@@ -3322,6 +4005,9 @@
         <v>1719864</v>
       </c>
       <c r="C228">
+        <v>2066349.175621891</v>
+      </c>
+      <c r="D228">
         <v>-346485.1756218907</v>
       </c>
     </row>
@@ -3335,6 +4021,9 @@
         <v>7500000</v>
       </c>
       <c r="C229">
+        <v>7219039.347844115</v>
+      </c>
+      <c r="D229">
         <v>280960.6521558855</v>
       </c>
     </row>
@@ -3348,6 +4037,9 @@
         <v>25000000</v>
       </c>
       <c r="C230">
+        <v>12948284.02470979</v>
+      </c>
+      <c r="D230">
         <v>12051715.97529021</v>
       </c>
     </row>
@@ -3361,6 +4053,9 @@
         <v>2019706</v>
       </c>
       <c r="C231">
+        <v>2686171.174295192</v>
+      </c>
+      <c r="D231">
         <v>-666465.1742951917</v>
       </c>
     </row>
@@ -3374,6 +4069,9 @@
         <v>3835738</v>
       </c>
       <c r="C232">
+        <v>5597203.349585407</v>
+      </c>
+      <c r="D232">
         <v>-1761465.349585407</v>
       </c>
     </row>
@@ -3387,6 +4085,9 @@
         <v>29682540</v>
       </c>
       <c r="C233">
+        <v>22571708.020398</v>
+      </c>
+      <c r="D233">
         <v>7110831.979601998</v>
       </c>
     </row>
@@ -3400,6 +4101,9 @@
         <v>8000000</v>
       </c>
       <c r="C234">
+        <v>5914627.796517414</v>
+      </c>
+      <c r="D234">
         <v>2085372.203482586</v>
       </c>
     </row>
@@ -3413,6 +4117,9 @@
         <v>2019706</v>
       </c>
       <c r="C235">
+        <v>3278839.931260365</v>
+      </c>
+      <c r="D235">
         <v>-1259133.931260365</v>
       </c>
     </row>
@@ -3426,6 +4133,9 @@
         <v>10576923</v>
       </c>
       <c r="C236">
+        <v>9742386.783499168</v>
+      </c>
+      <c r="D236">
         <v>834536.2165008318</v>
       </c>
     </row>
@@ -3439,6 +4149,9 @@
         <v>3191400</v>
       </c>
       <c r="C237">
+        <v>3808710.073217247</v>
+      </c>
+      <c r="D237">
         <v>-617310.0732172471</v>
       </c>
     </row>
@@ -3452,6 +4165,9 @@
         <v>2019706</v>
       </c>
       <c r="C238">
+        <v>4446108.073134328</v>
+      </c>
+      <c r="D238">
         <v>-2426402.073134328</v>
       </c>
     </row>
@@ -3465,6 +4181,9 @@
         <v>17259999</v>
       </c>
       <c r="C239">
+        <v>24809898.48946932</v>
+      </c>
+      <c r="D239">
         <v>-7549899.489469323</v>
       </c>
     </row>
@@ -3478,6 +4197,9 @@
         <v>1930681</v>
       </c>
       <c r="C240">
+        <v>2983735.644444444</v>
+      </c>
+      <c r="D240">
         <v>-1053054.644444444</v>
       </c>
     </row>
@@ -3491,6 +4213,9 @@
         <v>6802950</v>
       </c>
       <c r="C241">
+        <v>8209184.505721396</v>
+      </c>
+      <c r="D241">
         <v>-1406234.505721396</v>
       </c>
     </row>
@@ -3504,6 +4229,9 @@
         <v>7560000</v>
       </c>
       <c r="C242">
+        <v>6197906.653482586</v>
+      </c>
+      <c r="D242">
         <v>1362093.346517414</v>
       </c>
     </row>
@@ -3517,6 +4245,9 @@
         <v>1930681</v>
       </c>
       <c r="C243">
+        <v>1893394.996517413</v>
+      </c>
+      <c r="D243">
         <v>37286.00348258694</v>
       </c>
     </row>
@@ -3530,6 +4261,9 @@
         <v>2000000</v>
       </c>
       <c r="C244">
+        <v>3256320.148922056</v>
+      </c>
+      <c r="D244">
         <v>-1256320.148922056</v>
       </c>
     </row>
@@ -3543,6 +4277,9 @@
         <v>6916080</v>
       </c>
       <c r="C245">
+        <v>7331003.036069652</v>
+      </c>
+      <c r="D245">
         <v>-414923.0360696521</v>
       </c>
     </row>
@@ -3556,6 +4293,9 @@
         <v>2019706</v>
       </c>
       <c r="C246">
+        <v>5069282.210364842</v>
+      </c>
+      <c r="D246">
         <v>-3049576.210364842</v>
       </c>
     </row>
@@ -3569,6 +4309,9 @@
         <v>4343920</v>
       </c>
       <c r="C247">
+        <v>24249315.80306799</v>
+      </c>
+      <c r="D247">
         <v>-19905395.80306799</v>
       </c>
     </row>
@@ -3582,6 +4325,9 @@
         <v>1799163</v>
       </c>
       <c r="C248">
+        <v>4134696.628689884</v>
+      </c>
+      <c r="D248">
         <v>-2335533.628689884</v>
       </c>
     </row>
@@ -3595,6 +4341,9 @@
         <v>1836096</v>
       </c>
       <c r="C249">
+        <v>1958457.29344942</v>
+      </c>
+      <c r="D249">
         <v>-122361.29344942</v>
       </c>
     </row>
@@ -3608,6 +4357,9 @@
         <v>35802469</v>
       </c>
       <c r="C250">
+        <v>30243267.81177447</v>
+      </c>
+      <c r="D250">
         <v>5559201.188225526</v>
       </c>
     </row>
@@ -3621,6 +4373,9 @@
         <v>8700000</v>
       </c>
       <c r="C251">
+        <v>8923632.381426206</v>
+      </c>
+      <c r="D251">
         <v>-223632.3814262059</v>
       </c>
     </row>
@@ -3634,6 +4389,9 @@
         <v>3901399</v>
       </c>
       <c r="C252">
+        <v>6365162.443200663</v>
+      </c>
+      <c r="D252">
         <v>-2463763.443200663</v>
       </c>
     </row>
@@ -3647,6 +4405,9 @@
         <v>4516000</v>
       </c>
       <c r="C253">
+        <v>3939342.454560529</v>
+      </c>
+      <c r="D253">
         <v>576657.5454394706</v>
       </c>
     </row>
@@ -3660,6 +4421,9 @@
         <v>13750000</v>
       </c>
       <c r="C254">
+        <v>12615311.02852405</v>
+      </c>
+      <c r="D254">
         <v>1134688.971475951</v>
       </c>
     </row>
@@ -3673,6 +4437,9 @@
         <v>4368030</v>
       </c>
       <c r="C255">
+        <v>5102960.140215589</v>
+      </c>
+      <c r="D255">
         <v>-734930.1402155887</v>
       </c>
     </row>
@@ -3686,6 +4453,9 @@
         <v>1719864</v>
       </c>
       <c r="C256">
+        <v>2978564.840215588</v>
+      </c>
+      <c r="D256">
         <v>-1258700.840215588</v>
       </c>
     </row>
@@ -3699,6 +4469,9 @@
         <v>2320000</v>
       </c>
       <c r="C257">
+        <v>2785869.4039801</v>
+      </c>
+      <c r="D257">
         <v>-465869.4039800996</v>
       </c>
     </row>
@@ -3712,6 +4485,9 @@
         <v>8000000</v>
       </c>
       <c r="C258">
+        <v>9936547.189635158</v>
+      </c>
+      <c r="D258">
         <v>-1936547.189635158</v>
       </c>
     </row>
@@ -3725,6 +4501,9 @@
         <v>1997238</v>
       </c>
       <c r="C259">
+        <v>2942993.013432836</v>
+      </c>
+      <c r="D259">
         <v>-945755.0134328362</v>
       </c>
     </row>
@@ -3738,6 +4517,9 @@
         <v>2019706</v>
       </c>
       <c r="C260">
+        <v>4035550.35</v>
+      </c>
+      <c r="D260">
         <v>-2015844.35</v>
       </c>
     </row>
@@ -3751,6 +4533,9 @@
         <v>7723000</v>
       </c>
       <c r="C261">
+        <v>7748233.681674958</v>
+      </c>
+      <c r="D261">
         <v>-25233.68167495821</v>
       </c>
     </row>
@@ -3764,6 +4549,9 @@
         <v>29320988</v>
       </c>
       <c r="C262">
+        <v>16310957.31401327</v>
+      </c>
+      <c r="D262">
         <v>13010030.68598673</v>
       </c>
     </row>
@@ -3777,6 +4565,9 @@
         <v>10880400</v>
       </c>
       <c r="C263">
+        <v>10449190.45058043</v>
+      </c>
+      <c r="D263">
         <v>431209.5494195689</v>
       </c>
     </row>
@@ -3790,6 +4581,9 @@
         <v>1800000</v>
       </c>
       <c r="C264">
+        <v>2193848.37039801</v>
+      </c>
+      <c r="D264">
         <v>-393848.3703980097</v>
       </c>
     </row>
@@ -3803,6 +4597,9 @@
         <v>2966040</v>
       </c>
       <c r="C265">
+        <v>3537168.528938639</v>
+      </c>
+      <c r="D265">
         <v>-571128.5289386385</v>
       </c>
     </row>
@@ -3816,6 +4613,9 @@
         <v>6802950</v>
       </c>
       <c r="C266">
+        <v>6109447.265422887</v>
+      </c>
+      <c r="D266">
         <v>693502.7345771128</v>
       </c>
     </row>
@@ -3829,6 +4629,9 @@
         <v>5000000</v>
       </c>
       <c r="C267">
+        <v>4869649.782172471</v>
+      </c>
+      <c r="D267">
         <v>130350.2178275287</v>
       </c>
     </row>
@@ -3842,6 +4645,9 @@
         <v>1719864</v>
       </c>
       <c r="C268">
+        <v>1910617.564262024</v>
+      </c>
+      <c r="D268">
         <v>-190753.5642620237</v>
       </c>
     </row>
@@ -3855,6 +4661,9 @@
         <v>5063640</v>
       </c>
       <c r="C269">
+        <v>4973742.454809288</v>
+      </c>
+      <c r="D269">
         <v>89897.54519071244</v>
       </c>
     </row>
@@ -3868,6 +4677,9 @@
         <v>33162030</v>
       </c>
       <c r="C270">
+        <v>33242067.42470977</v>
+      </c>
+      <c r="D270">
         <v>-80037.42470977455</v>
       </c>
     </row>
@@ -3881,6 +4693,9 @@
         <v>8882640</v>
       </c>
       <c r="C271">
+        <v>16487360.94386401</v>
+      </c>
+      <c r="D271">
         <v>-7604720.943864014</v>
       </c>
     </row>
@@ -3894,6 +4709,9 @@
         <v>9945830</v>
       </c>
       <c r="C272">
+        <v>11718701.41782753</v>
+      </c>
+      <c r="D272">
         <v>-1772871.417827534</v>
       </c>
     </row>
@@ -3907,6 +4725,9 @@
         <v>3918480</v>
       </c>
       <c r="C273">
+        <v>3584524.686898839</v>
+      </c>
+      <c r="D273">
         <v>333955.3131011608</v>
       </c>
     </row>
@@ -3920,6 +4741,9 @@
         <v>2421720</v>
       </c>
       <c r="C274">
+        <v>2063764.648092869</v>
+      </c>
+      <c r="D274">
         <v>357955.351907131</v>
       </c>
     </row>
@@ -3933,6 +4757,9 @@
         <v>34005250</v>
       </c>
       <c r="C275">
+        <v>32039723.02280265</v>
+      </c>
+      <c r="D275">
         <v>1965526.977197353</v>
       </c>
     </row>
@@ -3946,6 +4773,9 @@
         <v>17116279</v>
       </c>
       <c r="C276">
+        <v>12538905.3247927</v>
+      </c>
+      <c r="D276">
         <v>4577373.675207296</v>
       </c>
     </row>
@@ -3959,6 +4789,9 @@
         <v>2019706</v>
       </c>
       <c r="C277">
+        <v>5688253.938225538</v>
+      </c>
+      <c r="D277">
         <v>-3668547.938225538</v>
       </c>
     </row>
@@ -3972,6 +4805,9 @@
         <v>3359280</v>
       </c>
       <c r="C278">
+        <v>13460122.63756219</v>
+      </c>
+      <c r="D278">
         <v>-10100842.63756219</v>
       </c>
     </row>
@@ -3985,6 +4821,9 @@
         <v>18214000</v>
       </c>
       <c r="C279">
+        <v>22477301.17810945</v>
+      </c>
+      <c r="D279">
         <v>-4263301.178109448</v>
       </c>
     </row>
@@ -3998,6 +4837,9 @@
         <v>33833400</v>
       </c>
       <c r="C280">
+        <v>29342759.02470978</v>
+      </c>
+      <c r="D280">
         <v>4490640.975290217</v>
       </c>
     </row>
@@ -4011,6 +4853,9 @@
         <v>8409000</v>
       </c>
       <c r="C281">
+        <v>13141332.4800995</v>
+      </c>
+      <c r="D281">
         <v>-4732332.480099499</v>
       </c>
     </row>
@@ -4024,6 +4869,9 @@
         <v>2847480</v>
       </c>
       <c r="C282">
+        <v>3144168.345936981</v>
+      </c>
+      <c r="D282">
         <v>-296688.3459369815</v>
       </c>
     </row>
@@ -4037,6 +4885,9 @@
         <v>3500000</v>
       </c>
       <c r="C283">
+        <v>5016726.608208954</v>
+      </c>
+      <c r="D283">
         <v>-1516726.608208954</v>
       </c>
     </row>
@@ -4050,6 +4901,9 @@
         <v>2019706</v>
       </c>
       <c r="C284">
+        <v>2307146.097595356</v>
+      </c>
+      <c r="D284">
         <v>-287440.0975953564</v>
       </c>
     </row>
@@ -4063,6 +4917,9 @@
         <v>10375000</v>
       </c>
       <c r="C285">
+        <v>8842224.819983415</v>
+      </c>
+      <c r="D285">
         <v>1532775.180016585</v>
       </c>
     </row>
@@ -4076,6 +4933,9 @@
         <v>2131905</v>
       </c>
       <c r="C286">
+        <v>7231933.214510782</v>
+      </c>
+      <c r="D286">
         <v>-5100028.214510782</v>
       </c>
     </row>
@@ -4089,6 +4949,9 @@
         <v>5634257</v>
       </c>
       <c r="C287">
+        <v>6594053.492703155</v>
+      </c>
+      <c r="D287">
         <v>-959796.4927031547</v>
       </c>
     </row>
@@ -4102,6 +4965,9 @@
         <v>8800000</v>
       </c>
       <c r="C288">
+        <v>7879009.012603647</v>
+      </c>
+      <c r="D288">
         <v>920990.9873963529</v>
       </c>
     </row>
@@ -4115,6 +4981,9 @@
         <v>4306281</v>
       </c>
       <c r="C289">
+        <v>3362850.789054725</v>
+      </c>
+      <c r="D289">
         <v>943430.2109452747</v>
       </c>
     </row>
@@ -4128,6 +4997,9 @@
         <v>16875000</v>
       </c>
       <c r="C290">
+        <v>19776042.34361525</v>
+      </c>
+      <c r="D290">
         <v>-2901042.343615249</v>
       </c>
     </row>
@@ -4141,6 +5013,9 @@
         <v>3000000</v>
       </c>
       <c r="C291">
+        <v>3558738.252238806</v>
+      </c>
+      <c r="D291">
         <v>-558738.2522388063</v>
       </c>
     </row>
@@ -4154,6 +5029,9 @@
         <v>9500000</v>
       </c>
       <c r="C292">
+        <v>9132256.052238801</v>
+      </c>
+      <c r="D292">
         <v>367743.9477611985</v>
       </c>
     </row>
@@ -4167,6 +5045,9 @@
         <v>5266713</v>
       </c>
       <c r="C293">
+        <v>2741720.29809287</v>
+      </c>
+      <c r="D293">
         <v>2524992.70190713</v>
       </c>
     </row>
@@ -4180,6 +5061,9 @@
         <v>2815937</v>
       </c>
       <c r="C294">
+        <v>3097835.815008292</v>
+      </c>
+      <c r="D294">
         <v>-281898.815008292</v>
       </c>
     </row>
@@ -4193,6 +5077,9 @@
         <v>8109063</v>
       </c>
       <c r="C295">
+        <v>6734405.282006633</v>
+      </c>
+      <c r="D295">
         <v>1374657.717993367</v>
       </c>
     </row>
@@ -4206,6 +5093,9 @@
         <v>8920795</v>
       </c>
       <c r="C296">
+        <v>8271494.11641791</v>
+      </c>
+      <c r="D296">
         <v>649300.88358209</v>
       </c>
     </row>
@@ -4219,6 +5109,9 @@
         <v>12195122</v>
       </c>
       <c r="C297">
+        <v>11699959.98665009</v>
+      </c>
+      <c r="D297">
         <v>495162.0133499149</v>
       </c>
     </row>
@@ -4232,6 +5125,9 @@
         <v>6718842</v>
       </c>
       <c r="C298">
+        <v>6385897.78499171</v>
+      </c>
+      <c r="D298">
         <v>332944.2150082905</v>
       </c>
     </row>
@@ -4245,6 +5141,9 @@
         <v>2019706</v>
       </c>
       <c r="C299">
+        <v>6241772.547844114</v>
+      </c>
+      <c r="D299">
         <v>-4222066.547844114</v>
       </c>
     </row>
@@ -4258,6 +5157,9 @@
         <v>30800000</v>
       </c>
       <c r="C300">
+        <v>25412065.53723051</v>
+      </c>
+      <c r="D300">
         <v>5387934.46276949</v>
       </c>
     </row>
@@ -4271,6 +5173,9 @@
         <v>8519706</v>
       </c>
       <c r="C301">
+        <v>7768417.412354893</v>
+      </c>
+      <c r="D301">
         <v>751288.5876451069</v>
       </c>
     </row>
@@ -4284,6 +5189,9 @@
         <v>8715000</v>
       </c>
       <c r="C302">
+        <v>8095670.20273632</v>
+      </c>
+      <c r="D302">
         <v>619329.79726368</v>
       </c>
     </row>
@@ -4297,6 +5205,9 @@
         <v>559782</v>
       </c>
       <c r="C303">
+        <v>2033302.679850747</v>
+      </c>
+      <c r="D303">
         <v>-1473520.679850747</v>
       </c>
     </row>
@@ -4310,6 +5221,9 @@
         <v>1600000</v>
       </c>
       <c r="C304">
+        <v>2378510.797595357</v>
+      </c>
+      <c r="D304">
         <v>-778510.7975953571</v>
       </c>
     </row>
@@ -4323,6 +5237,9 @@
         <v>1708143</v>
       </c>
       <c r="C305">
+        <v>2062420.783333334</v>
+      </c>
+      <c r="D305">
         <v>-354277.7833333337</v>
       </c>
     </row>
@@ -4336,6 +5253,9 @@
         <v>5000000</v>
       </c>
       <c r="C306">
+        <v>6176703.618076285</v>
+      </c>
+      <c r="D306">
         <v>-1176703.618076285</v>
       </c>
     </row>
@@ -4349,6 +5269,9 @@
         <v>3352440</v>
       </c>
       <c r="C307">
+        <v>5011179.420149253</v>
+      </c>
+      <c r="D307">
         <v>-1658739.420149253</v>
       </c>
     </row>
@@ -4362,6 +5285,9 @@
         <v>19500000</v>
       </c>
       <c r="C308">
+        <v>11445394.58905473</v>
+      </c>
+      <c r="D308">
         <v>8054605.410945274</v>
       </c>
     </row>
@@ -4375,6 +5301,9 @@
         <v>5009633</v>
       </c>
       <c r="C309">
+        <v>2720539.456799337</v>
+      </c>
+      <c r="D309">
         <v>2289093.543200663</v>
       </c>
     </row>
@@ -4388,6 +5317,9 @@
         <v>27455357</v>
       </c>
       <c r="C310">
+        <v>16441069.87819237</v>
+      </c>
+      <c r="D310">
         <v>11014287.12180763</v>
       </c>
     </row>
@@ -4401,6 +5333,9 @@
         <v>33386850</v>
       </c>
       <c r="C311">
+        <v>26521997.2566335</v>
+      </c>
+      <c r="D311">
         <v>6864852.743366499</v>
       </c>
     </row>
@@ -4414,6 +5349,9 @@
         <v>6300000</v>
       </c>
       <c r="C312">
+        <v>5771233.155887231</v>
+      </c>
+      <c r="D312">
         <v>528766.8441127688</v>
       </c>
     </row>
@@ -4427,6 +5365,9 @@
         <v>11710818</v>
       </c>
       <c r="C313">
+        <v>10051240.74170813</v>
+      </c>
+      <c r="D313">
         <v>1659577.258291874</v>
       </c>
     </row>
@@ -4440,6 +5381,9 @@
         <v>36016200</v>
       </c>
       <c r="C314">
+        <v>30918376.28150912</v>
+      </c>
+      <c r="D314">
         <v>5097823.718490876</v>
       </c>
     </row>
@@ -4453,6 +5397,9 @@
         <v>4000000</v>
       </c>
       <c r="C315">
+        <v>5896458.031260365</v>
+      </c>
+      <c r="D315">
         <v>-1896458.031260365</v>
       </c>
     </row>
@@ -4466,6 +5413,9 @@
         <v>18000000</v>
       </c>
       <c r="C316">
+        <v>14895675.57827528</v>
+      </c>
+      <c r="D316">
         <v>3104324.421724718</v>
       </c>
     </row>
@@ -4479,6 +5429,9 @@
         <v>6105941</v>
       </c>
       <c r="C317">
+        <v>5622578.331840798</v>
+      </c>
+      <c r="D317">
         <v>483362.6681592017</v>
       </c>
     </row>
@@ -4492,6 +5445,9 @@
         <v>4516000</v>
       </c>
       <c r="C318">
+        <v>7696124.739386396</v>
+      </c>
+      <c r="D318">
         <v>-3180124.739386396</v>
       </c>
     </row>
@@ -4505,6 +5461,9 @@
         <v>4037277</v>
       </c>
       <c r="C319">
+        <v>5081327.06119403</v>
+      </c>
+      <c r="D319">
         <v>-1044050.06119403</v>
       </c>
     </row>
@@ -4518,6 +5477,9 @@
         <v>2733720</v>
       </c>
       <c r="C320">
+        <v>3296820.848590382</v>
+      </c>
+      <c r="D320">
         <v>-563100.8485903819</v>
       </c>
     </row>
@@ -4531,6 +5493,9 @@
         <v>4171548</v>
       </c>
       <c r="C321">
+        <v>12379516.65149254</v>
+      </c>
+      <c r="D321">
         <v>-8207968.651492536</v>
       </c>
     </row>
@@ -4544,6 +5509,9 @@
         <v>28226880</v>
       </c>
       <c r="C322">
+        <v>31123276.50995025</v>
+      </c>
+      <c r="D322">
         <v>-2896396.50995025</v>
       </c>
     </row>
@@ -4557,6 +5525,9 @@
         <v>12015150</v>
       </c>
       <c r="C323">
+        <v>16911527.88913765</v>
+      </c>
+      <c r="D323">
         <v>-4896377.889137648</v>
       </c>
     </row>
@@ -4570,6 +5541,9 @@
         <v>2165000</v>
       </c>
       <c r="C324">
+        <v>4173615.810199005</v>
+      </c>
+      <c r="D324">
         <v>-2008615.810199005</v>
       </c>
     </row>
@@ -4583,6 +5557,9 @@
         <v>7723000</v>
       </c>
       <c r="C325">
+        <v>5386424.667330016</v>
+      </c>
+      <c r="D325">
         <v>2336575.332669984</v>
       </c>
     </row>
@@ -4596,6 +5573,9 @@
         <v>12950400</v>
       </c>
       <c r="C326">
+        <v>6990691.361774461</v>
+      </c>
+      <c r="D326">
         <v>5959708.638225539</v>
       </c>
     </row>
@@ -4609,6 +5589,9 @@
         <v>5000000</v>
       </c>
       <c r="C327">
+        <v>6042537.904311774</v>
+      </c>
+      <c r="D327">
         <v>-1042537.904311774</v>
       </c>
     </row>
@@ -4622,6 +5605,9 @@
         <v>2891467</v>
       </c>
       <c r="C328">
+        <v>8018121.609121061</v>
+      </c>
+      <c r="D328">
         <v>-5126654.609121061</v>
       </c>
     </row>
@@ -4635,6 +5621,9 @@
         <v>18154000</v>
       </c>
       <c r="C329">
+        <v>16075430.34063017</v>
+      </c>
+      <c r="D329">
         <v>2078569.659369826</v>
       </c>
     </row>
@@ -4648,6 +5637,9 @@
         <v>15681818</v>
       </c>
       <c r="C330">
+        <v>11814982.42578773</v>
+      </c>
+      <c r="D330">
         <v>3866835.574212268</v>
       </c>
     </row>
@@ -4661,6 +5653,9 @@
         <v>1801769</v>
       </c>
       <c r="C331">
+        <v>2338372.860613599</v>
+      </c>
+      <c r="D331">
         <v>-536603.860613599</v>
       </c>
     </row>
@@ -4674,6 +5669,9 @@
         <v>2718240</v>
       </c>
       <c r="C332">
+        <v>3696070.391542288</v>
+      </c>
+      <c r="D332">
         <v>-977830.391542288</v>
       </c>
     </row>
@@ -4687,6 +5685,9 @@
         <v>1719864</v>
       </c>
       <c r="C333">
+        <v>4018654.077114428</v>
+      </c>
+      <c r="D333">
         <v>-2298790.077114428</v>
       </c>
     </row>
@@ -4700,6 +5701,9 @@
         <v>3196448</v>
       </c>
       <c r="C334">
+        <v>5319497.878358209</v>
+      </c>
+      <c r="D334">
         <v>-2123049.878358209</v>
       </c>
     </row>
@@ -4713,6 +5717,9 @@
         <v>23205221</v>
       </c>
       <c r="C335">
+        <v>27815743.27222223</v>
+      </c>
+      <c r="D335">
         <v>-4610522.272222228</v>
       </c>
     </row>
@@ -4726,6 +5733,9 @@
         <v>1119563</v>
       </c>
       <c r="C336">
+        <v>1963678.671641791</v>
+      </c>
+      <c r="D336">
         <v>-844115.671641791</v>
       </c>
     </row>
@@ -4739,6 +5749,9 @@
         <v>17307693</v>
       </c>
       <c r="C337">
+        <v>19894056.96575455</v>
+      </c>
+      <c r="D337">
         <v>-2586363.965754554</v>
       </c>
     </row>
@@ -4752,6 +5765,9 @@
         <v>30600000</v>
       </c>
       <c r="C338">
+        <v>31553059.74676616</v>
+      </c>
+      <c r="D338">
         <v>-953059.7467661612</v>
       </c>
     </row>
@@ -4765,6 +5781,9 @@
         <v>2066585</v>
       </c>
       <c r="C339">
+        <v>2363860.909618573</v>
+      </c>
+      <c r="D339">
         <v>-297275.9096185728</v>
       </c>
     </row>
@@ -4778,6 +5797,9 @@
         <v>1029483</v>
       </c>
       <c r="C340">
+        <v>1725893.60721393</v>
+      </c>
+      <c r="D340">
         <v>-696410.6072139305</v>
       </c>
     </row>
@@ -4791,6 +5813,9 @@
         <v>2019706</v>
       </c>
       <c r="C341">
+        <v>4740010.917910447</v>
+      </c>
+      <c r="D341">
         <v>-2720304.917910447</v>
       </c>
     </row>
@@ -4804,6 +5829,9 @@
         <v>2624040</v>
       </c>
       <c r="C342">
+        <v>3758454.913432836</v>
+      </c>
+      <c r="D342">
         <v>-1134414.913432836</v>
       </c>
     </row>
@@ -4817,6 +5845,9 @@
         <v>12405000</v>
       </c>
       <c r="C343">
+        <v>16771381.75290215</v>
+      </c>
+      <c r="D343">
         <v>-4366381.752902152</v>
       </c>
     </row>
@@ -4830,6 +5861,9 @@
         <v>3536280</v>
       </c>
       <c r="C344">
+        <v>12904425.93897181</v>
+      </c>
+      <c r="D344">
         <v>-9368145.938971814</v>
       </c>
     </row>
@@ -4843,6 +5877,9 @@
         <v>2448600</v>
       </c>
       <c r="C345">
+        <v>2578480.79145937</v>
+      </c>
+      <c r="D345">
         <v>-129880.7914593699</v>
       </c>
     </row>
@@ -4856,6 +5893,9 @@
         <v>17325000</v>
       </c>
       <c r="C346">
+        <v>15512863.60480928</v>
+      </c>
+      <c r="D346">
         <v>1812136.395190716</v>
       </c>
     </row>
@@ -4869,6 +5909,9 @@
         <v>10250000</v>
       </c>
       <c r="C347">
+        <v>7177285.751990051</v>
+      </c>
+      <c r="D347">
         <v>3072714.248009949</v>
       </c>
     </row>
@@ -4882,6 +5925,9 @@
         <v>2210040</v>
       </c>
       <c r="C348">
+        <v>3105300.502736319</v>
+      </c>
+      <c r="D348">
         <v>-895260.5027363189</v>
       </c>
     </row>
@@ -4895,6 +5941,9 @@
         <v>6313800</v>
       </c>
       <c r="C349">
+        <v>8853353.941873964</v>
+      </c>
+      <c r="D349">
         <v>-2539553.941873964</v>
       </c>
     </row>
@@ -4908,6 +5957,9 @@
         <v>2537160</v>
       </c>
       <c r="C350">
+        <v>3008409.489220565</v>
+      </c>
+      <c r="D350">
         <v>-471249.4892205647</v>
       </c>
     </row>
@@ -4921,6 +5973,9 @@
         <v>37893408</v>
       </c>
       <c r="C351">
+        <v>29367948.21393036</v>
+      </c>
+      <c r="D351">
         <v>8525459.786069639</v>
       </c>
     </row>
@@ -4934,6 +5989,9 @@
         <v>37893408</v>
       </c>
       <c r="C352">
+        <v>29362677.75787728</v>
+      </c>
+      <c r="D352">
         <v>8530730.242122725</v>
       </c>
     </row>
@@ -4947,6 +6005,9 @@
         <v>24107143</v>
       </c>
       <c r="C353">
+        <v>24416363.95903814</v>
+      </c>
+      <c r="D353">
         <v>-309220.9590381421</v>
       </c>
     </row>
@@ -4960,6 +6021,9 @@
         <v>1927896</v>
       </c>
       <c r="C354">
+        <v>2334371.314096187</v>
+      </c>
+      <c r="D354">
         <v>-406475.3140961868</v>
       </c>
     </row>
@@ -4973,6 +6037,9 @@
         <v>18833713</v>
       </c>
       <c r="C355">
+        <v>18930521.01492538</v>
+      </c>
+      <c r="D355">
         <v>-96808.01492537931</v>
       </c>
     </row>
@@ -4986,6 +6053,9 @@
         <v>2019706</v>
       </c>
       <c r="C356">
+        <v>3774258.945522387</v>
+      </c>
+      <c r="D356">
         <v>-1754552.945522387</v>
       </c>
     </row>
@@ -4999,6 +6069,9 @@
         <v>1801769</v>
       </c>
       <c r="C357">
+        <v>3072863.670149253</v>
+      </c>
+      <c r="D357">
         <v>-1271094.670149253</v>
       </c>
     </row>
@@ -5012,6 +6085,9 @@
         <v>2019706</v>
       </c>
       <c r="C358">
+        <v>8745093.363267001</v>
+      </c>
+      <c r="D358">
         <v>-6725387.363267001</v>
       </c>
     </row>
@@ -5025,6 +6101,9 @@
         <v>9326520</v>
       </c>
       <c r="C359">
+        <v>9012373.155472636</v>
+      </c>
+      <c r="D359">
         <v>314146.8445273638</v>
       </c>
     </row>
@@ -5038,6 +6117,9 @@
         <v>5043773</v>
       </c>
       <c r="C360">
+        <v>5158911.337147596</v>
+      </c>
+      <c r="D360">
         <v>-115138.3371475963</v>
       </c>
     </row>
@@ -5051,6 +6133,9 @@
         <v>2463960</v>
       </c>
       <c r="C361">
+        <v>3334827.316086235</v>
+      </c>
+      <c r="D361">
         <v>-870867.3160862345</v>
       </c>
     </row>
@@ -5064,6 +6149,9 @@
         <v>5316960</v>
       </c>
       <c r="C362">
+        <v>8038219.577529022</v>
+      </c>
+      <c r="D362">
         <v>-2721259.577529022</v>
       </c>
     </row>
@@ -5077,6 +6165,9 @@
         <v>2226240</v>
       </c>
       <c r="C363">
+        <v>2669075.896766169</v>
+      </c>
+      <c r="D363">
         <v>-442835.896766169</v>
       </c>
     </row>
@@ -5090,6 +6181,9 @@
         <v>2419706</v>
       </c>
       <c r="C364">
+        <v>2392178.512437811</v>
+      </c>
+      <c r="D364">
         <v>27527.48756218934</v>
       </c>
     </row>
@@ -5103,6 +6197,9 @@
         <v>5266713</v>
       </c>
       <c r="C365">
+        <v>8841987.340878936</v>
+      </c>
+      <c r="D365">
         <v>-3575274.340878936</v>
       </c>
     </row>
@@ -5116,6 +6213,9 @@
         <v>2431080</v>
       </c>
       <c r="C366">
+        <v>3056151.674709786</v>
+      </c>
+      <c r="D366">
         <v>-625071.6747097857</v>
       </c>
     </row>
@@ -5129,6 +6229,9 @@
         <v>14487684</v>
       </c>
       <c r="C367">
+        <v>17877731.55497513</v>
+      </c>
+      <c r="D367">
         <v>-3390047.554975126</v>
       </c>
     </row>
@@ -5142,6 +6245,9 @@
         <v>7252080</v>
       </c>
       <c r="C368">
+        <v>8215266.947678279</v>
+      </c>
+      <c r="D368">
         <v>-963186.9476782791</v>
       </c>
     </row>
@@ -5155,6 +6261,9 @@
         <v>6500000</v>
       </c>
       <c r="C369">
+        <v>6021623.397927036</v>
+      </c>
+      <c r="D369">
         <v>478376.6020729644</v>
       </c>
     </row>
@@ -5168,6 +6277,9 @@
         <v>32600060</v>
       </c>
       <c r="C370">
+        <v>32042380.2066335</v>
+      </c>
+      <c r="D370">
         <v>557679.793366503</v>
       </c>
     </row>
@@ -5181,6 +6293,9 @@
         <v>2019706</v>
       </c>
       <c r="C371">
+        <v>2276146.339054727</v>
+      </c>
+      <c r="D371">
         <v>-256440.339054727</v>
       </c>
     </row>
@@ -5194,6 +6309,9 @@
         <v>2019706</v>
       </c>
       <c r="C372">
+        <v>3148167.384411278</v>
+      </c>
+      <c r="D372">
         <v>-1128461.384411278</v>
       </c>
     </row>
@@ -5207,6 +6325,9 @@
         <v>3350760</v>
       </c>
       <c r="C373">
+        <v>3242770.544776118</v>
+      </c>
+      <c r="D373">
         <v>107989.4552238816</v>
       </c>
     </row>
@@ -5220,6 +6341,9 @@
         <v>8670002</v>
       </c>
       <c r="C374">
+        <v>7335223.847678277</v>
+      </c>
+      <c r="D374">
         <v>1334778.152321723</v>
       </c>
     </row>
@@ -5233,6 +6357,9 @@
         <v>8670002</v>
       </c>
       <c r="C375">
+        <v>8441178.633582087</v>
+      </c>
+      <c r="D375">
         <v>228823.3664179128</v>
       </c>
     </row>
@@ -5246,6 +6373,9 @@
         <v>2240160</v>
       </c>
       <c r="C376">
+        <v>9651625.139054727</v>
+      </c>
+      <c r="D376">
         <v>-7411465.139054727</v>
       </c>
     </row>
@@ -5259,6 +6389,9 @@
         <v>8809320</v>
       </c>
       <c r="C377">
+        <v>6417339.764925373</v>
+      </c>
+      <c r="D377">
         <v>2391980.235074627</v>
       </c>
     </row>
@@ -5272,6 +6405,9 @@
         <v>7977480</v>
       </c>
       <c r="C378">
+        <v>8031357.72238806</v>
+      </c>
+      <c r="D378">
         <v>-53877.72238805983</v>
       </c>
     </row>
@@ -5285,6 +6421,9 @@
         <v>43219440</v>
       </c>
       <c r="C379">
+        <v>33209873.50912106</v>
+      </c>
+      <c r="D379">
         <v>10009566.49087894</v>
       </c>
     </row>
@@ -5298,6 +6437,9 @@
         <v>2019706</v>
       </c>
       <c r="C380">
+        <v>3790962.182918741</v>
+      </c>
+      <c r="D380">
         <v>-1771256.182918741</v>
       </c>
     </row>
@@ -5311,6 +6453,9 @@
         <v>1836096</v>
       </c>
       <c r="C381">
+        <v>3743972.275124377</v>
+      </c>
+      <c r="D381">
         <v>-1907876.275124377</v>
       </c>
     </row>
@@ -5324,6 +6469,9 @@
         <v>10500000</v>
       </c>
       <c r="C382">
+        <v>8847781.504394695</v>
+      </c>
+      <c r="D382">
         <v>1652218.495605305</v>
       </c>
     </row>
@@ -5337,6 +6485,9 @@
         <v>1930681</v>
       </c>
       <c r="C383">
+        <v>2837276.490298508</v>
+      </c>
+      <c r="D383">
         <v>-906595.4902985077</v>
       </c>
     </row>
@@ -5350,6 +6501,9 @@
         <v>6803012</v>
       </c>
       <c r="C384">
+        <v>7967528.832006632</v>
+      </c>
+      <c r="D384">
         <v>-1164516.832006632</v>
       </c>
     </row>
@@ -5363,6 +6517,9 @@
         <v>36016200</v>
       </c>
       <c r="C385">
+        <v>33291223.24527363</v>
+      </c>
+      <c r="D385">
         <v>2724976.754726373</v>
       </c>
     </row>
@@ -5376,6 +6533,9 @@
         <v>18560000</v>
       </c>
       <c r="C386">
+        <v>9068215.335903814</v>
+      </c>
+      <c r="D386">
         <v>9491784.664096186</v>
       </c>
     </row>
@@ -5389,6 +6549,9 @@
         <v>11014500</v>
       </c>
       <c r="C387">
+        <v>9468191.437810943</v>
+      </c>
+      <c r="D387">
         <v>1546308.562189057</v>
       </c>
     </row>
@@ -5402,6 +6565,9 @@
         <v>20975000</v>
       </c>
       <c r="C388">
+        <v>21481419.92968491</v>
+      </c>
+      <c r="D388">
         <v>-506419.9296849146</v>
       </c>
     </row>
@@ -5415,6 +6581,9 @@
         <v>1119563</v>
       </c>
       <c r="C389">
+        <v>1506195.681757877</v>
+      </c>
+      <c r="D389">
         <v>-386632.6817578771</v>
       </c>
     </row>
@@ -5428,6 +6597,9 @@
         <v>15435000</v>
       </c>
       <c r="C390">
+        <v>21244213.75588723</v>
+      </c>
+      <c r="D390">
         <v>-5809213.755887225</v>
       </c>
     </row>
@@ -5441,6 +6613,9 @@
         <v>4698000</v>
       </c>
       <c r="C391">
+        <v>4611690.210364842</v>
+      </c>
+      <c r="D391">
         <v>86309.78963515814</v>
       </c>
     </row>
@@ -5454,6 +6629,9 @@
         <v>40806300</v>
       </c>
       <c r="C392">
+        <v>32301660.22271974</v>
+      </c>
+      <c r="D392">
         <v>8504639.777280264</v>
       </c>
     </row>
@@ -5467,6 +6645,9 @@
         <v>5887899</v>
       </c>
       <c r="C393">
+        <v>10933405.5655058</v>
+      </c>
+      <c r="D393">
         <v>-5045506.565505803</v>
       </c>
     </row>
@@ -5480,6 +6661,9 @@
         <v>6341464</v>
       </c>
       <c r="C394">
+        <v>5587225.67039801</v>
+      </c>
+      <c r="D394">
         <v>754238.3296019901</v>
       </c>
     </row>
@@ -5493,6 +6677,9 @@
         <v>10500000</v>
       </c>
       <c r="C395">
+        <v>9487318.523880595</v>
+      </c>
+      <c r="D395">
         <v>1012681.476119405</v>
       </c>
     </row>
@@ -5506,6 +6693,9 @@
         <v>18518519</v>
       </c>
       <c r="C396">
+        <v>24086574.98225541</v>
+      </c>
+      <c r="D396">
         <v>-5568055.98225541</v>
       </c>
     </row>
@@ -5519,6 +6709,9 @@
         <v>5709877</v>
       </c>
       <c r="C397">
+        <v>5740452.722222223</v>
+      </c>
+      <c r="D397">
         <v>-30575.72222222295</v>
       </c>
     </row>
@@ -5532,6 +6725,9 @@
         <v>5508720</v>
       </c>
       <c r="C398">
+        <v>10093527.44883914</v>
+      </c>
+      <c r="D398">
         <v>-4584807.448839137</v>
       </c>
     </row>
@@ -5545,6 +6741,9 @@
         <v>8000000</v>
       </c>
       <c r="C399">
+        <v>7607970.713432835</v>
+      </c>
+      <c r="D399">
         <v>392029.2865671646</v>
       </c>
     </row>
@@ -5558,6 +6757,9 @@
         <v>1927896</v>
       </c>
       <c r="C400">
+        <v>2643110.724958541</v>
+      </c>
+      <c r="D400">
         <v>-715214.7249585409</v>
       </c>
     </row>
@@ -5571,6 +6773,9 @@
         <v>1719864</v>
       </c>
       <c r="C401">
+        <v>4232561.710447761</v>
+      </c>
+      <c r="D401">
         <v>-2512697.710447761</v>
       </c>
     </row>
@@ -5584,6 +6789,9 @@
         <v>6059520</v>
       </c>
       <c r="C402">
+        <v>4984893.821144278</v>
+      </c>
+      <c r="D402">
         <v>1074626.178855722</v>
       </c>
     </row>
@@ -5597,6 +6805,9 @@
         <v>2019706</v>
       </c>
       <c r="C403">
+        <v>6559909.899004975</v>
+      </c>
+      <c r="D403">
         <v>-4540203.899004975</v>
       </c>
     </row>
@@ -5610,6 +6821,9 @@
         <v>5291400</v>
       </c>
       <c r="C404">
+        <v>4367477.711359868</v>
+      </c>
+      <c r="D404">
         <v>923922.2886401322</v>
       </c>
     </row>
@@ -5623,6 +6837,9 @@
         <v>16847826</v>
       </c>
       <c r="C405">
+        <v>16560930.01409618</v>
+      </c>
+      <c r="D405">
         <v>286895.9859038163</v>
       </c>
     </row>
@@ -5636,6 +6853,9 @@
         <v>2346614</v>
       </c>
       <c r="C406">
+        <v>4151505.880845771</v>
+      </c>
+      <c r="D406">
         <v>-1804891.880845771</v>
       </c>
     </row>
@@ -5649,6 +6869,9 @@
         <v>2019706</v>
       </c>
       <c r="C407">
+        <v>3247057.38888889</v>
+      </c>
+      <c r="D407">
         <v>-1227351.38888889</v>
       </c>
     </row>
@@ -5662,6 +6885,9 @@
         <v>2303520</v>
       </c>
       <c r="C408">
+        <v>2818542.04742952</v>
+      </c>
+      <c r="D408">
         <v>-515022.0474295197</v>
       </c>
     </row>
@@ -5675,6 +6901,9 @@
         <v>12160680</v>
       </c>
       <c r="C409">
+        <v>11855595.69237148</v>
+      </c>
+      <c r="D409">
         <v>305084.3076285217</v>
       </c>
     </row>
@@ -5688,6 +6917,9 @@
         <v>2504640</v>
       </c>
       <c r="C410">
+        <v>3577835.778524048</v>
+      </c>
+      <c r="D410">
         <v>-1073195.778524048</v>
       </c>
     </row>
@@ -5701,6 +6933,9 @@
         <v>3835738</v>
       </c>
       <c r="C411">
+        <v>9431284.709286898</v>
+      </c>
+      <c r="D411">
         <v>-5595546.709286898</v>
       </c>
     </row>
@@ -5714,6 +6949,9 @@
         <v>11111111</v>
       </c>
       <c r="C412">
+        <v>17217348.08756219</v>
+      </c>
+      <c r="D412">
         <v>-6106237.087562189</v>
       </c>
     </row>
@@ -5727,6 +6965,9 @@
         <v>18357143</v>
       </c>
       <c r="C413">
+        <v>22377318.48905472</v>
+      </c>
+      <c r="D413">
         <v>-4020175.489054721</v>
       </c>
     </row>
@@ -5740,6 +6981,9 @@
         <v>3218160</v>
       </c>
       <c r="C414">
+        <v>3548998.816749585</v>
+      </c>
+      <c r="D414">
         <v>-330838.8167495853</v>
       </c>
     </row>
@@ -5753,6 +6997,9 @@
         <v>1836096</v>
       </c>
       <c r="C415">
+        <v>2523986.396185737</v>
+      </c>
+      <c r="D415">
         <v>-687890.3961857366</v>
       </c>
     </row>
@@ -5766,6 +7013,9 @@
         <v>24330357</v>
       </c>
       <c r="C416">
+        <v>10810324.36575456</v>
+      </c>
+      <c r="D416">
         <v>13520032.63424544</v>
       </c>
     </row>
@@ -5779,6 +7029,9 @@
         <v>12405000</v>
       </c>
       <c r="C417">
+        <v>10056893.90887231</v>
+      </c>
+      <c r="D417">
         <v>2348106.091127692</v>
       </c>
     </row>
@@ -5792,6 +7045,9 @@
         <v>4558680</v>
       </c>
       <c r="C418">
+        <v>8764119.722885573</v>
+      </c>
+      <c r="D418">
         <v>-4205439.722885573</v>
       </c>
     </row>
@@ -5805,6 +7061,9 @@
         <v>2000000</v>
       </c>
       <c r="C419">
+        <v>3109303.239635157</v>
+      </c>
+      <c r="D419">
         <v>-1109303.239635157</v>
       </c>
     </row>
@@ -5818,6 +7077,9 @@
         <v>6175000</v>
       </c>
       <c r="C420">
+        <v>6149778.44660033</v>
+      </c>
+      <c r="D420">
         <v>25221.55339966994</v>
       </c>
     </row>
@@ -5831,6 +7093,9 @@
         <v>3908160</v>
       </c>
       <c r="C421">
+        <v>6236092.373631842</v>
+      </c>
+      <c r="D421">
         <v>-2327932.373631842</v>
       </c>
     </row>
@@ -5844,6 +7109,9 @@
         <v>9835881</v>
       </c>
       <c r="C422">
+        <v>7085261.761359867</v>
+      </c>
+      <c r="D422">
         <v>2750619.238640133</v>
       </c>
     </row>
@@ -5857,6 +7125,9 @@
         <v>11571429</v>
       </c>
       <c r="C423">
+        <v>8065711.60456053</v>
+      </c>
+      <c r="D423">
         <v>3505717.39543947</v>
       </c>
     </row>
@@ -5870,6 +7141,9 @@
         <v>4810200</v>
       </c>
       <c r="C424">
+        <v>3458484.992039802</v>
+      </c>
+      <c r="D424">
         <v>1351715.007960198</v>
       </c>
     </row>
@@ -5883,6 +7157,9 @@
         <v>34005250</v>
       </c>
       <c r="C425">
+        <v>26454253.61517414</v>
+      </c>
+      <c r="D425">
         <v>7550996.384825859</v>
       </c>
     </row>
@@ -5896,6 +7173,9 @@
         <v>2019706</v>
       </c>
       <c r="C426">
+        <v>1974467.033830847</v>
+      </c>
+      <c r="D426">
         <v>45238.96616915287</v>
       </c>
     </row>
@@ -5909,6 +7189,9 @@
         <v>12119440</v>
       </c>
       <c r="C427">
+        <v>5725611.755389719</v>
+      </c>
+      <c r="D427">
         <v>6393828.244610281</v>
       </c>
     </row>
@@ -5922,6 +7205,9 @@
         <v>2709849</v>
       </c>
       <c r="C428">
+        <v>3915435.556550581</v>
+      </c>
+      <c r="D428">
         <v>-1205586.556550581</v>
       </c>
     </row>
@@ -5935,6 +7221,9 @@
         <v>8195122</v>
       </c>
       <c r="C429">
+        <v>8179408.876036484</v>
+      </c>
+      <c r="D429">
         <v>15713.12396351621</v>
       </c>
     </row>
@@ -5948,6 +7237,9 @@
         <v>8000000</v>
       </c>
       <c r="C430">
+        <v>5918718.626119401</v>
+      </c>
+      <c r="D430">
         <v>2081281.373880599</v>
       </c>
     </row>
@@ -5961,6 +7253,9 @@
         <v>40064220</v>
       </c>
       <c r="C431">
+        <v>35805973.99237148</v>
+      </c>
+      <c r="D431">
         <v>4258246.007628515</v>
       </c>
     </row>
@@ -5974,6 +7269,9 @@
         <v>2800000</v>
       </c>
       <c r="C432">
+        <v>3566424.322388059</v>
+      </c>
+      <c r="D432">
         <v>-766424.3223880595</v>
       </c>
     </row>
@@ -5987,6 +7285,9 @@
         <v>2019706</v>
       </c>
       <c r="C433">
+        <v>3877711.316169154</v>
+      </c>
+      <c r="D433">
         <v>-1858005.316169154</v>
       </c>
     </row>
@@ -6000,6 +7301,9 @@
         <v>10933333</v>
       </c>
       <c r="C434">
+        <v>11586401.94411277</v>
+      </c>
+      <c r="D434">
         <v>-653068.9441127665</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new column to see the percent of total salary for the residual
</commit_message>
<xml_diff>
--- a/residualTable.xlsx
+++ b/residualTable.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D434"/>
+  <dimension ref="A1:E434"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,17 +365,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Current Year Salary</t>
+          <t>Current.Year.Salary</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Predicted Salary</t>
+          <t>Predicted.Salary</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Residual</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Percent.of.Salary.Off</t>
         </is>
       </c>
     </row>
@@ -394,6 +399,9 @@
       <c r="D2">
         <v>480012.3093698169</v>
       </c>
+      <c r="E2">
+        <v>0.1096036876516156</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -410,6 +418,9 @@
       <c r="D3">
         <v>699210.1972636804</v>
       </c>
+      <c r="E3">
+        <v>0.02144812608515691</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -426,6 +437,9 @@
       <c r="D4">
         <v>560830.2565505793</v>
       </c>
+      <c r="E4">
+        <v>0.1363157494897135</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -442,6 +456,9 @@
       <c r="D5">
         <v>-5250635.821227196</v>
       </c>
+      <c r="E5">
+        <v>-2.392961362331235</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -458,6 +475,9 @@
       <c r="D6">
         <v>707313.5830845754</v>
       </c>
+      <c r="E6">
+        <v>0.1508935643913761</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -474,6 +494,9 @@
       <c r="D7">
         <v>-6883175.850165844</v>
       </c>
+      <c r="E7">
+        <v>-0.7712241848925315</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -490,6 +513,9 @@
       <c r="D8">
         <v>700945.5833333395</v>
       </c>
+      <c r="E8">
+        <v>0.03504727916666698</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -506,6 +532,9 @@
       <c r="D9">
         <v>-868467.4142620238</v>
       </c>
+      <c r="E9">
+        <v>-0.4729967356075193</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -522,6 +551,9 @@
       <c r="D10">
         <v>-1518256.80588723</v>
       </c>
+      <c r="E10">
+        <v>-0.1646786517428721</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -538,6 +570,9 @@
       <c r="D11">
         <v>3427221.500995025</v>
       </c>
+      <c r="E11">
+        <v>0.07509235743288784</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -554,6 +589,9 @@
       <c r="D12">
         <v>-1041576.498590381</v>
       </c>
+      <c r="E12">
+        <v>-0.5157069883390855</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -570,6 +608,9 @@
       <c r="D13">
         <v>-1793289.723714761</v>
       </c>
+      <c r="E13">
+        <v>-0.3237118869561144</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -586,6 +627,9 @@
       <c r="D14">
         <v>-88889.55232173204</v>
       </c>
+      <c r="E14">
+        <v>-0.004768022000154378</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -602,6 +646,9 @@
       <c r="D15">
         <v>-151806.6234660042</v>
       </c>
+      <c r="E15">
+        <v>-0.0751627333215845</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -618,6 +665,9 @@
       <c r="D16">
         <v>-1417814.686567168</v>
       </c>
+      <c r="E16">
+        <v>-0.2263726853747912</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -634,6 +684,9 @@
       <c r="D17">
         <v>6522250.419900507</v>
       </c>
+      <c r="E17">
+        <v>0.2009354080591447</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -650,6 +703,9 @@
       <c r="D18">
         <v>3449719.801326701</v>
       </c>
+      <c r="E18">
+        <v>0.2759775841061361</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -666,6 +722,9 @@
       <c r="D19">
         <v>-294453.3963515759</v>
       </c>
+      <c r="E19">
+        <v>-0.1259575125984189</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -682,6 +741,9 @@
       <c r="D20">
         <v>-2988273.483416259</v>
       </c>
+      <c r="E20">
+        <v>-0.274137560189499</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -698,6 +760,9 @@
       <c r="D21">
         <v>-572539.0560530671</v>
       </c>
+      <c r="E21">
+        <v>-0.2834764347152838</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -714,6 +779,9 @@
       <c r="D22">
         <v>-1156203.968988394</v>
       </c>
+      <c r="E22">
+        <v>-0.09960337704326593</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -730,6 +798,9 @@
       <c r="D23">
         <v>-15104761.13076285</v>
       </c>
+      <c r="E23">
+        <v>-3.928331620088006</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -746,6 +817,9 @@
       <c r="D24">
         <v>-218767.1587893856</v>
       </c>
+      <c r="E24">
+        <v>-0.1083163385113406</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -762,6 +836,9 @@
       <c r="D25">
         <v>2796024.067081254</v>
       </c>
+      <c r="E25">
+        <v>0.1644720039459561</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -778,6 +855,9 @@
       <c r="D26">
         <v>-4761869.658540631</v>
       </c>
+      <c r="E26">
+        <v>-0.5945885787096788</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -794,6 +874,9 @@
       <c r="D27">
         <v>5109478.860613603</v>
       </c>
+      <c r="E27">
+        <v>0.2139295783626556</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -810,6 +893,9 @@
       <c r="D28">
         <v>-1752024.693781096</v>
       </c>
+      <c r="E28">
+        <v>-0.6738556514542675</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -826,6 +912,9 @@
       <c r="D29">
         <v>-2866601.098092868</v>
       </c>
+      <c r="E29">
+        <v>-1.221590384312404</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -842,6 +931,9 @@
       <c r="D30">
         <v>2188290.723217251</v>
       </c>
+      <c r="E30">
+        <v>0.1868606209418719</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -858,6 +950,9 @@
       <c r="D31">
         <v>13347620.53383085</v>
       </c>
+      <c r="E31">
+        <v>0.2855619702673967</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -874,6 +969,9 @@
       <c r="D32">
         <v>-5086931.991625208</v>
       </c>
+      <c r="E32">
+        <v>-2.518649739925122</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -890,6 +988,9 @@
       <c r="D33">
         <v>-842416.0700663342</v>
       </c>
+      <c r="E33">
+        <v>-0.3228389936638055</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -906,6 +1007,9 @@
       <c r="D34">
         <v>5595267.431094525</v>
       </c>
+      <c r="E34">
+        <v>0.329133378299678</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -922,6 +1026,9 @@
       <c r="D35">
         <v>-2950577.560613598</v>
       </c>
+      <c r="E35">
+        <v>-1.46089458595142</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -938,6 +1045,9 @@
       <c r="D36">
         <v>-4194448.871227197</v>
       </c>
+      <c r="E36">
+        <v>-0.9204442656966676</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -954,6 +1064,9 @@
       <c r="D37">
         <v>-1548760.372885573</v>
       </c>
+      <c r="E37">
+        <v>-0.7494297949929827</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -970,6 +1083,9 @@
       <c r="D38">
         <v>-3351812.898756221</v>
       </c>
+      <c r="E38">
+        <v>-0.6703625797512441</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -986,6 +1102,9 @@
       <c r="D39">
         <v>2725833.017495854</v>
       </c>
+      <c r="E39">
+        <v>0.3762115163516915</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1002,6 +1121,9 @@
       <c r="D40">
         <v>-1288404.148756217</v>
       </c>
+      <c r="E40">
+        <v>-0.06889861758054637</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1018,6 +1140,9 @@
       <c r="D41">
         <v>-1586046.495356549</v>
       </c>
+      <c r="E41">
+        <v>-0.07930232476782743</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1034,6 +1159,9 @@
       <c r="D42">
         <v>49843.64286898798</v>
       </c>
+      <c r="E42">
+        <v>0.02467866257217039</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1050,6 +1178,9 @@
       <c r="D43">
         <v>1948800.296102822</v>
       </c>
+      <c r="E43">
+        <v>0.05410899251178142</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1066,6 +1197,9 @@
       <c r="D44">
         <v>-758580.1192371473</v>
       </c>
+      <c r="E44">
+        <v>-0.413148397053938</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1082,6 +1216,9 @@
       <c r="D45">
         <v>2197033.571144281</v>
       </c>
+      <c r="E45">
+        <v>0.1869815805229175</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1098,6 +1235,9 @@
       <c r="D46">
         <v>708313.7859867327</v>
       </c>
+      <c r="E46">
+        <v>0.154989362546549</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1114,6 +1254,9 @@
       <c r="D47">
         <v>-1313140.288308457</v>
       </c>
+      <c r="E47">
+        <v>-0.427471219028236</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1130,6 +1273,9 @@
       <c r="D48">
         <v>-543610.9912106148</v>
       </c>
+      <c r="E48">
+        <v>-0.1843298988208736</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1146,6 +1292,9 @@
       <c r="D49">
         <v>-5288240.72363184</v>
       </c>
+      <c r="E49">
+        <v>-0.243697729199624</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1162,6 +1311,9 @@
       <c r="D50">
         <v>-8572497.061194031</v>
       </c>
+      <c r="E50">
+        <v>-1.08220835736483</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1178,6 +1330,9 @@
       <c r="D51">
         <v>-467103.9819237143</v>
       </c>
+      <c r="E51">
+        <v>-0.2157524165929396</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1194,6 +1349,9 @@
       <c r="D52">
         <v>-165456.9117744677</v>
       </c>
+      <c r="E52">
+        <v>-0.007353640523309675</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1210,6 +1368,9 @@
       <c r="D53">
         <v>4913325.298756219</v>
       </c>
+      <c r="E53">
+        <v>0.2171379148457753</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1226,6 +1387,9 @@
       <c r="D54">
         <v>9229144.523631843</v>
       </c>
+      <c r="E54">
+        <v>0.4195065692559928</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1242,6 +1406,9 @@
       <c r="D55">
         <v>1809222.491127688</v>
       </c>
+      <c r="E55">
+        <v>0.05683952872811601</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1258,6 +1425,9 @@
       <c r="D56">
         <v>-433804.2970978436</v>
       </c>
+      <c r="E56">
+        <v>-0.1797541548977523</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1274,6 +1444,9 @@
       <c r="D57">
         <v>-2479632.606301823</v>
       </c>
+      <c r="E57">
+        <v>-1.227719582108397</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1290,6 +1463,9 @@
       <c r="D58">
         <v>807354.2718076278</v>
       </c>
+      <c r="E58">
+        <v>0.2018385679519069</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1306,6 +1482,9 @@
       <c r="D59">
         <v>-2234702.210696515</v>
       </c>
+      <c r="E59">
+        <v>-0.08481916500161785</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1322,6 +1501,9 @@
       <c r="D60">
         <v>-670889.6858208957</v>
       </c>
+      <c r="E60">
+        <v>-0.2653591207063968</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1338,6 +1520,9 @@
       <c r="D61">
         <v>1139155.160779436</v>
       </c>
+      <c r="E61">
+        <v>0.2782308881609064</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1354,6 +1539,9 @@
       <c r="D62">
         <v>3306721.035903813</v>
       </c>
+      <c r="E62">
+        <v>0.2537037999475987</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1370,6 +1558,9 @@
       <c r="D63">
         <v>32031.82064676844</v>
       </c>
+      <c r="E63">
+        <v>0.003053674176972281</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1386,6 +1577,9 @@
       <c r="D64">
         <v>5404682.380265325</v>
       </c>
+      <c r="E64">
+        <v>0.1196150665029211</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1402,6 +1596,9 @@
       <c r="D65">
         <v>2483127.647429518</v>
       </c>
+      <c r="E65">
+        <v>0.1688635237652494</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1418,6 +1615,9 @@
       <c r="D66">
         <v>-2307221.338225538</v>
       </c>
+      <c r="E66">
+        <v>-2.060823141016217</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1434,6 +1634,9 @@
       <c r="D67">
         <v>4347572.738142623</v>
       </c>
+      <c r="E67">
+        <v>0.210883427344908</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1450,6 +1653,9 @@
       <c r="D68">
         <v>-488228.5864013284</v>
       </c>
+      <c r="E68">
+        <v>-0.07886769715306681</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1466,6 +1672,9 @@
       <c r="D69">
         <v>3188635.738142623</v>
       </c>
+      <c r="E69">
+        <v>0.2443399033059481</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1482,6 +1691,9 @@
       <c r="D70">
         <v>497022.3509121072</v>
       </c>
+      <c r="E70">
+        <v>0.05253936056153353</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1498,6 +1710,9 @@
       <c r="D71">
         <v>-810858.0984245446</v>
       </c>
+      <c r="E71">
+        <v>-0.2702860328081815</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1514,6 +1729,9 @@
       <c r="D72">
         <v>-1006493.195605306</v>
       </c>
+      <c r="E72">
+        <v>-0.5852167355124047</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1530,6 +1748,9 @@
       <c r="D73">
         <v>-1376427.912686567</v>
       </c>
+      <c r="E73">
+        <v>-1.229433191956654</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1546,6 +1767,9 @@
       <c r="D74">
         <v>-86225.3477612175</v>
       </c>
+      <c r="E74">
+        <v>-0.003671096293338825</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1562,6 +1786,9 @@
       <c r="D75">
         <v>-165947.5868159179</v>
       </c>
+      <c r="E75">
+        <v>-0.01724130772113432</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1578,6 +1805,9 @@
       <c r="D76">
         <v>-4464.922305141576</v>
       </c>
+      <c r="E76">
+        <v>-0.001445183169275996</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1594,6 +1824,9 @@
       <c r="D77">
         <v>-251524.8553067981</v>
       </c>
+      <c r="E77">
+        <v>-0.06859768157479207</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1610,6 +1843,9 @@
       <c r="D78">
         <v>3398230.980514094</v>
       </c>
+      <c r="E78">
+        <v>0.1341054057030029</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1626,6 +1862,9 @@
       <c r="D79">
         <v>-2297366.924378112</v>
       </c>
+      <c r="E79">
+        <v>-0.2983593408283262</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1642,6 +1881,9 @@
       <c r="D80">
         <v>2000933.292868994</v>
       </c>
+      <c r="E80">
+        <v>0.08214011875488482</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1658,6 +1900,9 @@
       <c r="D81">
         <v>1657038.846268654</v>
       </c>
+      <c r="E81">
+        <v>0.1758342402964912</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1674,6 +1919,9 @@
       <c r="D82">
         <v>-115103.969485906</v>
       </c>
+      <c r="E82">
+        <v>-0.01740234303445061</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1690,6 +1938,9 @@
       <c r="D83">
         <v>2319148.830845775</v>
       </c>
+      <c r="E83">
+        <v>0.1983482500500137</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1706,6 +1957,9 @@
       <c r="D84">
         <v>-2915786.728358208</v>
       </c>
+      <c r="E84">
+        <v>-1.153290352731812</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1722,6 +1976,9 @@
       <c r="D85">
         <v>-3560673.43026534</v>
       </c>
+      <c r="E85">
+        <v>-1.762966209074657</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1738,6 +1995,9 @@
       <c r="D86">
         <v>-2141240.52064677</v>
       </c>
+      <c r="E86">
+        <v>-0.193683473052598</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1754,6 +2014,9 @@
       <c r="D87">
         <v>-3864160.211276948</v>
       </c>
+      <c r="E87">
+        <v>-0.9660400528192369</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1770,6 +2033,9 @@
       <c r="D88">
         <v>8516069.81807626</v>
       </c>
+      <c r="E88">
+        <v>0.1640367704028212</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1786,6 +2052,9 @@
       <c r="D89">
         <v>944912.1976782745</v>
       </c>
+      <c r="E89">
+        <v>0.1633631732533686</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1802,6 +2071,9 @@
       <c r="D90">
         <v>3122291.414676607</v>
       </c>
+      <c r="E90">
+        <v>0.07690357789138856</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1818,6 +2090,9 @@
       <c r="D91">
         <v>1636985.960779437</v>
       </c>
+      <c r="E91">
+        <v>0.324104292543644</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1834,6 +2109,9 @@
       <c r="D92">
         <v>-1339983.154726364</v>
       </c>
+      <c r="E92">
+        <v>-0.04685255785756517</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1850,6 +2128,9 @@
       <c r="D93">
         <v>722587.242703151</v>
       </c>
+      <c r="E93">
+        <v>0.1592752567280218</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1866,6 +2147,9 @@
       <c r="D94">
         <v>856481.7222222215</v>
       </c>
+      <c r="E94">
+        <v>0.1784917019327576</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1882,6 +2166,9 @@
       <c r="D95">
         <v>-2220223.418490879</v>
       </c>
+      <c r="E95">
+        <v>-0.1090636057570003</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1898,6 +2185,9 @@
       <c r="D96">
         <v>4828357.986152572</v>
       </c>
+      <c r="E96">
+        <v>0.4429686225828047</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1914,6 +2204,9 @@
       <c r="D97">
         <v>2855733.327446111</v>
       </c>
+      <c r="E97">
+        <v>0.07127889492035813</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1930,6 +2223,9 @@
       <c r="D98">
         <v>7087650.098092865</v>
       </c>
+      <c r="E98">
+        <v>0.4639189087636216</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1946,6 +2242,9 @@
       <c r="D99">
         <v>2531376.056965173</v>
       </c>
+      <c r="E99">
+        <v>0.3905551318302162</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1962,6 +2261,9 @@
       <c r="D100">
         <v>-4064288.259701491</v>
       </c>
+      <c r="E100">
+        <v>-1.209609601101634</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1978,6 +2280,9 @@
       <c r="D101">
         <v>376742.2032338302</v>
       </c>
+      <c r="E101">
+        <v>0.09134472971434152</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1994,6 +2299,9 @@
       <c r="D102">
         <v>-4481744.540215587</v>
       </c>
+      <c r="E102">
+        <v>-1.732634314925043</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2010,6 +2318,9 @@
       <c r="D103">
         <v>7769348.096932001</v>
       </c>
+      <c r="E103">
+        <v>0.1630522675250302</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2026,6 +2337,9 @@
       <c r="D104">
         <v>-3795296.704477613</v>
       </c>
+      <c r="E104">
+        <v>-0.8763743117657303</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2042,6 +2356,9 @@
       <c r="D105">
         <v>-1191121.38432836</v>
       </c>
+      <c r="E105">
+        <v>-0.3376998447273046</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2058,6 +2375,9 @@
       <c r="D106">
         <v>-2482544.502985081</v>
       </c>
+      <c r="E106">
+        <v>-0.1834191406492663</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2074,6 +2394,9 @@
       <c r="D107">
         <v>11967.32238805923</v>
       </c>
+      <c r="E107">
+        <v>0.006207452263015861</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2090,6 +2413,9 @@
       <c r="D108">
         <v>7240789.05953566</v>
       </c>
+      <c r="E108">
+        <v>0.1520939321246753</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2106,6 +2432,9 @@
       <c r="D109">
         <v>-638267.4712271988</v>
       </c>
+      <c r="E109">
+        <v>-0.2719950836512519</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2122,6 +2451,9 @@
       <c r="D110">
         <v>-1495568.202736318</v>
       </c>
+      <c r="E110">
+        <v>-0.4985227342454394</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2138,6 +2470,9 @@
       <c r="D111">
         <v>-62443.39071310032</v>
       </c>
+      <c r="E111">
+        <v>-0.02418859522138503</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2154,6 +2489,9 @@
       <c r="D112">
         <v>1577450.443615254</v>
       </c>
+      <c r="E112">
+        <v>0.1132249165816768</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2170,6 +2508,9 @@
       <c r="D113">
         <v>-185823.504145937</v>
       </c>
+      <c r="E113">
+        <v>-0.04797890644804437</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2186,6 +2527,9 @@
       <c r="D114">
         <v>-1257715.502155887</v>
       </c>
+      <c r="E114">
+        <v>-0.4130602213018764</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2202,6 +2546,9 @@
       <c r="D115">
         <v>5710319.065422883</v>
       </c>
+      <c r="E115">
+        <v>0.3028199481450018</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2218,6 +2565,9 @@
       <c r="D116">
         <v>1060010.45008292</v>
       </c>
+      <c r="E116">
+        <v>0.03251559813334456</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2234,6 +2584,9 @@
       <c r="D117">
         <v>2550572.85613599</v>
       </c>
+      <c r="E117">
+        <v>0.1500336974197641</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2250,6 +2603,9 @@
       <c r="D118">
         <v>3819629.235489219</v>
       </c>
+      <c r="E118">
+        <v>0.3079849407748121</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2266,6 +2622,9 @@
       <c r="D119">
         <v>-414186.857131009</v>
       </c>
+      <c r="E119">
+        <v>-0.06088341927119985</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2282,6 +2641,9 @@
       <c r="D120">
         <v>4061615.892288554</v>
       </c>
+      <c r="E120">
+        <v>0.1194408478775646</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2298,6 +2660,9 @@
       <c r="D121">
         <v>-2779516.265505807</v>
       </c>
+      <c r="E121">
+        <v>-0.7145653415357619</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2314,6 +2679,9 @@
       <c r="D122">
         <v>5188725.128109433</v>
       </c>
+      <c r="E122">
+        <v>0.1136878961070587</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2330,6 +2698,9 @@
       <c r="D123">
         <v>-2522206.218988394</v>
       </c>
+      <c r="E123">
+        <v>-0.3829043423128438</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2346,6 +2717,9 @@
       <c r="D124">
         <v>-310627.8575456045</v>
       </c>
+      <c r="E124">
+        <v>-0.1537985516434592</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2362,6 +2736,9 @@
       <c r="D125">
         <v>939787.2852404639</v>
       </c>
+      <c r="E125">
+        <v>0.02814842625885533</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2378,6 +2755,9 @@
       <c r="D126">
         <v>-1736911.63747927</v>
       </c>
+      <c r="E126">
+        <v>-0.869656814800875</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2394,6 +2774,9 @@
       <c r="D127">
         <v>19936133.94925373</v>
       </c>
+      <c r="E127">
+        <v>0.4862471694939934</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2410,6 +2793,9 @@
       <c r="D128">
         <v>-746522.3414593698</v>
       </c>
+      <c r="E128">
+        <v>-0.3872212720288697</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2426,6 +2812,9 @@
       <c r="D129">
         <v>1427446.705306798</v>
       </c>
+      <c r="E129">
+        <v>0.06410828337371886</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2442,6 +2831,9 @@
       <c r="D130">
         <v>-7073231.935240466</v>
       </c>
+      <c r="E130">
+        <v>-2.212841233531866</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2458,6 +2850,9 @@
       <c r="D131">
         <v>3232341.203233829</v>
       </c>
+      <c r="E131">
+        <v>0.267135636630895</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2474,6 +2869,9 @@
       <c r="D132">
         <v>1845748.786318399</v>
       </c>
+      <c r="E132">
+        <v>0.0669083932531355</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2490,6 +2888,9 @@
       <c r="D133">
         <v>-523809.5649253731</v>
       </c>
+      <c r="E133">
+        <v>-0.2754328022621954</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2506,6 +2907,9 @@
       <c r="D134">
         <v>-2565488.212769486</v>
       </c>
+      <c r="E134">
+        <v>-12.82744106384743</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2522,6 +2926,9 @@
       <c r="D135">
         <v>4180405.499917079</v>
       </c>
+      <c r="E135">
+        <v>0.1872821628004676</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2538,6 +2945,9 @@
       <c r="D136">
         <v>-362473.0813432857</v>
       </c>
+      <c r="E136">
+        <v>-0.03664497945133446</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2554,6 +2964,9 @@
       <c r="D137">
         <v>-112566.1184908804</v>
       </c>
+      <c r="E137">
+        <v>-0.01172563734280004</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2570,6 +2983,9 @@
       <c r="D138">
         <v>-248642.3415422896</v>
       </c>
+      <c r="E138">
+        <v>-0.05217726200429593</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2586,6 +3002,9 @@
       <c r="D139">
         <v>108144.361608624</v>
       </c>
+      <c r="E139">
+        <v>0.02912649925358585</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2602,6 +3021,9 @@
       <c r="D140">
         <v>-863800.9966832502</v>
       </c>
+      <c r="E140">
+        <v>-0.3620714068219448</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2618,6 +3040,9 @@
       <c r="D141">
         <v>-823875.9531509127</v>
       </c>
+      <c r="E141">
+        <v>-0.7358906583648376</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2634,6 +3059,9 @@
       <c r="D142">
         <v>4587820.879104478</v>
       </c>
+      <c r="E142">
+        <v>0.2914615569308001</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2650,6 +3078,9 @@
       <c r="D143">
         <v>-14627268.4973466</v>
       </c>
+      <c r="E143">
+        <v>-2.518280483012481</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2666,6 +3097,9 @@
       <c r="D144">
         <v>-2144921.610281926</v>
       </c>
+      <c r="E144">
+        <v>-0.1198432343078365</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2682,6 +3116,9 @@
       <c r="D145">
         <v>526272.2247097939</v>
       </c>
+      <c r="E145">
+        <v>0.01476633627131857</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2698,6 +3135,9 @@
       <c r="D146">
         <v>-2291496.934411278</v>
       </c>
+      <c r="E146">
+        <v>-1.332371009807333</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2714,6 +3154,9 @@
       <c r="D147">
         <v>5663816.326782756</v>
       </c>
+      <c r="E147">
+        <v>0.4356781789832889</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2730,6 +3173,9 @@
       <c r="D148">
         <v>5152113.378689885</v>
       </c>
+      <c r="E148">
+        <v>0.2585289923040586</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2746,6 +3192,9 @@
       <c r="D149">
         <v>12441397.31898839</v>
       </c>
+      <c r="E149">
+        <v>0.3168156301666377</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2762,6 +3211,9 @@
       <c r="D150">
         <v>870433.4817578811</v>
       </c>
+      <c r="E150">
+        <v>0.0671630772961328</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2778,6 +3230,9 @@
       <c r="D151">
         <v>4337628.120398008</v>
       </c>
+      <c r="E151">
+        <v>0.4691802433302937</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2794,6 +3249,9 @@
       <c r="D152">
         <v>-1714125.298590383</v>
       </c>
+      <c r="E152">
+        <v>-0.8891170989464071</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2810,6 +3268,9 @@
       <c r="D153">
         <v>-723569.4850746272</v>
       </c>
+      <c r="E153">
+        <v>-0.1678753190309936</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2826,6 +3287,9 @@
       <c r="D154">
         <v>-336374.7573797675</v>
       </c>
+      <c r="E154">
+        <v>-0.1553694029467748</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2842,6 +3306,9 @@
       <c r="D155">
         <v>-142700.5869817603</v>
       </c>
+      <c r="E155">
+        <v>-0.01924756583790438</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2858,6 +3325,9 @@
       <c r="D156">
         <v>5101800.737147592</v>
       </c>
+      <c r="E156">
+        <v>0.1619619281634156</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2874,6 +3344,9 @@
       <c r="D157">
         <v>-1023735.612023218</v>
       </c>
+      <c r="E157">
+        <v>-0.1047741464456853</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2890,6 +3363,9 @@
       <c r="D158">
         <v>872054.2081260365</v>
       </c>
+      <c r="E158">
+        <v>0.1565649431456891</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2906,6 +3382,9 @@
       <c r="D159">
         <v>-429952.2597844079</v>
       </c>
+      <c r="E159">
+        <v>-0.01592415776979289</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2922,6 +3401,9 @@
       <c r="D160">
         <v>2637192.877860704</v>
       </c>
+      <c r="E160">
+        <v>0.1367849910100765</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2938,6 +3420,9 @@
       <c r="D161">
         <v>-3413096.163515755</v>
       </c>
+      <c r="E161">
+        <v>-1.794348232285979</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2954,6 +3439,9 @@
       <c r="D162">
         <v>-1684477.609203981</v>
       </c>
+      <c r="E162">
+        <v>-0.8340211937796792</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2970,6 +3458,9 @@
       <c r="D163">
         <v>11183651.0376451</v>
       </c>
+      <c r="E163">
+        <v>0.3033948221021099</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2986,6 +3477,9 @@
       <c r="D164">
         <v>-7557412.626533996</v>
       </c>
+      <c r="E164">
+        <v>-3.741837983614445</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -3002,6 +3496,9 @@
       <c r="D165">
         <v>6566199.786152571</v>
       </c>
+      <c r="E165">
+        <v>0.5450928843014183</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -3018,6 +3515,9 @@
       <c r="D166">
         <v>428294.7079601977</v>
       </c>
+      <c r="E166">
+        <v>0.04123769574043883</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -3034,6 +3534,9 @@
       <c r="D167">
         <v>84170.84121061396</v>
       </c>
+      <c r="E167">
+        <v>0.02277941272912173</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -3050,6 +3553,9 @@
       <c r="D168">
         <v>-90199.6891376432</v>
       </c>
+      <c r="E168">
+        <v>-0.009019968913764321</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3066,6 +3572,9 @@
       <c r="D169">
         <v>1695161.489552233</v>
       </c>
+      <c r="E169">
+        <v>0.1538259064929431</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -3082,6 +3591,9 @@
       <c r="D170">
         <v>-1020561.186401328</v>
       </c>
+      <c r="E170">
+        <v>-0.2367754043040028</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3098,6 +3610,9 @@
       <c r="D171">
         <v>-600286.2365671638</v>
       </c>
+      <c r="E171">
+        <v>-0.3001431182835819</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -3114,6 +3629,9 @@
       <c r="D172">
         <v>1693001.680597015</v>
       </c>
+      <c r="E172">
+        <v>0.3367951143067189</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -3130,6 +3648,9 @@
       <c r="D173">
         <v>3906346.942371475</v>
       </c>
+      <c r="E173">
+        <v>0.2492939336506565</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3146,6 +3667,9 @@
       <c r="D174">
         <v>545104.9282752872</v>
       </c>
+      <c r="E174">
+        <v>0.02713411159935137</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3162,6 +3686,9 @@
       <c r="D175">
         <v>-1122031.28955224</v>
       </c>
+      <c r="E175">
+        <v>-0.4864859909609087</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3178,6 +3705,9 @@
       <c r="D176">
         <v>3647704.639137646</v>
       </c>
+      <c r="E176">
+        <v>0.3316095126488769</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3194,6 +3724,9 @@
       <c r="D177">
         <v>2193776.731343269</v>
       </c>
+      <c r="E177">
+        <v>0.0648405638021384</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -3210,6 +3743,9 @@
       <c r="D178">
         <v>6966168.912354898</v>
       </c>
+      <c r="E178">
+        <v>0.1880865608216688</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -3226,6 +3762,9 @@
       <c r="D179">
         <v>12387276.92404644</v>
       </c>
+      <c r="E179">
+        <v>0.7119124668992206</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -3242,6 +3781,9 @@
       <c r="D180">
         <v>-733729.8592868987</v>
       </c>
+      <c r="E180">
+        <v>-0.09635981173854272</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -3258,6 +3800,9 @@
       <c r="D181">
         <v>-917832.9266998344</v>
       </c>
+      <c r="E181">
+        <v>-0.819813558236414</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -3274,6 +3819,9 @@
       <c r="D182">
         <v>-517253.5219734665</v>
       </c>
+      <c r="E182">
+        <v>-0.191839690971808</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -3290,6 +3838,9 @@
       <c r="D183">
         <v>324777.0686567165</v>
       </c>
+      <c r="E183">
+        <v>0.01198341996922304</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -3306,6 +3857,9 @@
       <c r="D184">
         <v>-2224343.895688227</v>
       </c>
+      <c r="E184">
+        <v>-0.4448687791376455</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -3322,6 +3876,9 @@
       <c r="D185">
         <v>-979418.8325870656</v>
       </c>
+      <c r="E185">
+        <v>-0.8748224374930804</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -3338,6 +3895,9 @@
       <c r="D186">
         <v>10295051.1181592</v>
       </c>
+      <c r="E186">
+        <v>0.2162491950961185</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -3354,6 +3914,9 @@
       <c r="D187">
         <v>-3859989.179767828</v>
       </c>
+      <c r="E187">
+        <v>-1.099524064196385</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -3370,6 +3933,9 @@
       <c r="D188">
         <v>13164.32454394619</v>
       </c>
+      <c r="E188">
+        <v>0.006370086177895509</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -3386,6 +3952,9 @@
       <c r="D189">
         <v>-756689.8400497516</v>
       </c>
+      <c r="E189">
+        <v>-0.3102427568597089</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -3402,6 +3971,9 @@
       <c r="D190">
         <v>-1425618.949751243</v>
       </c>
+      <c r="E190">
+        <v>-0.7137952260828422</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -3418,6 +3990,9 @@
       <c r="D191">
         <v>4690537.872636817</v>
       </c>
+      <c r="E191">
+        <v>0.1826579815280675</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -3434,6 +4009,9 @@
       <c r="D192">
         <v>-4462324.720066336</v>
       </c>
+      <c r="E192">
+        <v>-1.52539336015613</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -3450,6 +4028,9 @@
       <c r="D193">
         <v>1202695.460116085</v>
       </c>
+      <c r="E193">
+        <v>0.06013477300580423</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -3466,6 +4047,9 @@
       <c r="D194">
         <v>6025586.771807633</v>
       </c>
+      <c r="E194">
+        <v>0.1265684137387952</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -3482,6 +4066,9 @@
       <c r="D195">
         <v>-50861.70787728066</v>
       </c>
+      <c r="E195">
+        <v>-0.02518272851458611</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -3498,6 +4085,9 @@
       <c r="D196">
         <v>-11612.64684908791</v>
       </c>
+      <c r="E196">
+        <v>-0.004489428220928456</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -3514,6 +4104,9 @@
       <c r="D197">
         <v>-1119132.839220564</v>
       </c>
+      <c r="E197">
+        <v>-0.2080286244676872</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -3530,6 +4123,9 @@
       <c r="D198">
         <v>1553064.618242126</v>
       </c>
+      <c r="E198">
+        <v>0.1292588622066413</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -3546,6 +4142,9 @@
       <c r="D199">
         <v>208497.7416252065</v>
       </c>
+      <c r="E199">
+        <v>0.02106924617919548</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -3562,6 +4161,9 @@
       <c r="D200">
         <v>-967186.946600331</v>
       </c>
+      <c r="E200">
+        <v>-0.06908478190002364</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -3578,6 +4180,9 @@
       <c r="D201">
         <v>-4104229.955389718</v>
       </c>
+      <c r="E201">
+        <v>-2.032092767655153</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -3594,6 +4199,9 @@
       <c r="D202">
         <v>-2124175.353067994</v>
       </c>
+      <c r="E202">
+        <v>-1.051725029815227</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -3610,6 +4218,9 @@
       <c r="D203">
         <v>-942690.0557213943</v>
       </c>
+      <c r="E203">
+        <v>-0.4008035951196404</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -3626,6 +4237,9 @@
       <c r="D204">
         <v>5184372.474046437</v>
       </c>
+      <c r="E204">
+        <v>0.3511582427287179</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -3642,6 +4256,9 @@
       <c r="D205">
         <v>-1587545.311359867</v>
       </c>
+      <c r="E205">
+        <v>-0.5607402306333328</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -3658,6 +4275,9 @@
       <c r="D206">
         <v>-1183297.901243782</v>
       </c>
+      <c r="E206">
+        <v>-0.3179164923654184</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -3674,6 +4294,9 @@
       <c r="D207">
         <v>2435691.560696514</v>
       </c>
+      <c r="E207">
+        <v>0.2214265055178649</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -3690,6 +4313,9 @@
       <c r="D208">
         <v>-2064096.572470977</v>
       </c>
+      <c r="E208">
+        <v>-1.118392068278855</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -3706,6 +4332,9 @@
       <c r="D209">
         <v>-1356256.886152571</v>
       </c>
+      <c r="E209">
+        <v>-0.5651070358969044</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -3722,6 +4351,9 @@
       <c r="D210">
         <v>3210975.40986733</v>
       </c>
+      <c r="E210">
+        <v>0.5979058072101793</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -3738,6 +4370,9 @@
       <c r="D211">
         <v>-1774007.43482587</v>
       </c>
+      <c r="E211">
+        <v>-0.7350948885121268</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -3754,6 +4389,9 @@
       <c r="D212">
         <v>234928.9362354875</v>
       </c>
+      <c r="E212">
+        <v>0.03907121031583868</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -3770,6 +4408,9 @@
       <c r="D213">
         <v>-2052778.172305141</v>
       </c>
+      <c r="E213">
+        <v>-0.08028643461256418</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -3786,6 +4427,9 @@
       <c r="D214">
         <v>1067950.709867329</v>
       </c>
+      <c r="E214">
+        <v>0.1334938387334162</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -3802,6 +4446,9 @@
       <c r="D215">
         <v>238709.7373963506</v>
       </c>
+      <c r="E215">
+        <v>0.07459865790280713</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -3818,6 +4465,9 @@
       <c r="D216">
         <v>6304493.769071303</v>
       </c>
+      <c r="E216">
+        <v>0.1573597032232577</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -3834,6 +4484,9 @@
       <c r="D217">
         <v>-1031353.139883915</v>
       </c>
+      <c r="E217">
+        <v>-0.5106451829543087</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -3850,6 +4503,9 @@
       <c r="D218">
         <v>6130324.388391368</v>
       </c>
+      <c r="E218">
+        <v>0.1343188673445774</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -3866,6 +4522,9 @@
       <c r="D219">
         <v>-3939652.03772803</v>
       </c>
+      <c r="E219">
+        <v>-0.256077372209227</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -3882,6 +4541,9 @@
       <c r="D220">
         <v>887457.5832504136</v>
       </c>
+      <c r="E220">
+        <v>0.1550925537424291</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -3898,6 +4560,9 @@
       <c r="D221">
         <v>-397154.7729684906</v>
       </c>
+      <c r="E221">
+        <v>-0.3547408881576924</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -3914,6 +4579,9 @@
       <c r="D222">
         <v>-189012.2368159203</v>
       </c>
+      <c r="E222">
+        <v>-0.1049037012047162</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -3930,6 +4598,9 @@
       <c r="D223">
         <v>5089774.036484241</v>
       </c>
+      <c r="E223">
+        <v>0.1115198218409116</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -3946,6 +4617,9 @@
       <c r="D224">
         <v>1146275.204145935</v>
       </c>
+      <c r="E224">
+        <v>0.1834040326633496</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -3962,6 +4636,9 @@
       <c r="D225">
         <v>-291786.6722222231</v>
       </c>
+      <c r="E225">
+        <v>-0.06109896730537125</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -3978,6 +4655,9 @@
       <c r="D226">
         <v>-4244290.498839137</v>
       </c>
+      <c r="E226">
+        <v>-2.311584197579613</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -3994,6 +4674,9 @@
       <c r="D227">
         <v>-557722.6308457709</v>
       </c>
+      <c r="E227">
+        <v>-0.4981610064335557</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -4010,6 +4693,9 @@
       <c r="D228">
         <v>-346485.1756218907</v>
       </c>
+      <c r="E228">
+        <v>-0.2014607990061369</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -4026,6 +4712,9 @@
       <c r="D229">
         <v>280960.6521558855</v>
       </c>
+      <c r="E229">
+        <v>0.0374614202874514</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -4042,6 +4731,9 @@
       <c r="D230">
         <v>12051715.97529021</v>
       </c>
+      <c r="E230">
+        <v>0.4820686390116085</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -4058,6 +4750,9 @@
       <c r="D231">
         <v>-666465.1742951917</v>
       </c>
+      <c r="E231">
+        <v>-0.3299812815801862</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -4074,6 +4769,9 @@
       <c r="D232">
         <v>-1761465.349585407</v>
       </c>
+      <c r="E232">
+        <v>-0.4592246262871467</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -4090,6 +4788,9 @@
       <c r="D233">
         <v>7110831.979601998</v>
       </c>
+      <c r="E233">
+        <v>0.2395627860554386</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -4106,6 +4807,9 @@
       <c r="D234">
         <v>2085372.203482586</v>
       </c>
+      <c r="E234">
+        <v>0.2606715254353232</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -4122,6 +4826,9 @@
       <c r="D235">
         <v>-1259133.931260365</v>
       </c>
+      <c r="E235">
+        <v>-0.6234243653583069</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -4138,6 +4845,9 @@
       <c r="D236">
         <v>834536.2165008318</v>
       </c>
+      <c r="E236">
+        <v>0.07890160649754487</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -4154,6 +4864,9 @@
       <c r="D237">
         <v>-617310.0732172471</v>
       </c>
+      <c r="E237">
+        <v>-0.193429238960095</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -4170,6 +4883,9 @@
       <c r="D238">
         <v>-2426402.073134328</v>
       </c>
+      <c r="E238">
+        <v>-1.201363997103701</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -4186,6 +4902,9 @@
       <c r="D239">
         <v>-7549899.489469323</v>
       </c>
+      <c r="E239">
+        <v>-0.437421780237028</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -4202,6 +4921,9 @@
       <c r="D240">
         <v>-1053054.644444444</v>
       </c>
+      <c r="E240">
+        <v>-0.5454317126674185</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -4218,6 +4940,9 @@
       <c r="D241">
         <v>-1406234.505721396</v>
       </c>
+      <c r="E241">
+        <v>-0.2067095165658127</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -4234,6 +4959,9 @@
       <c r="D242">
         <v>1362093.346517414</v>
       </c>
+      <c r="E242">
+        <v>0.1801710775816685</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -4250,6 +4978,9 @@
       <c r="D243">
         <v>37286.00348258694</v>
       </c>
+      <c r="E243">
+        <v>0.01931235842823695</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -4266,6 +4997,9 @@
       <c r="D244">
         <v>-1256320.148922056</v>
       </c>
+      <c r="E244">
+        <v>-0.628160074461028</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -4282,6 +5016,9 @@
       <c r="D245">
         <v>-414923.0360696521</v>
       </c>
+      <c r="E245">
+        <v>-0.05999396132919979</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -4298,6 +5035,9 @@
       <c r="D246">
         <v>-3049576.210364842</v>
       </c>
+      <c r="E246">
+        <v>-1.50991095256678</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -4314,6 +5054,9 @@
       <c r="D247">
         <v>-19905395.80306799</v>
       </c>
+      <c r="E247">
+        <v>-4.582357824975596</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -4330,6 +5073,9 @@
       <c r="D248">
         <v>-2335533.628689884</v>
       </c>
+      <c r="E248">
+        <v>-1.298122309479399</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -4346,6 +5092,9 @@
       <c r="D249">
         <v>-122361.29344942</v>
       </c>
+      <c r="E249">
+        <v>-0.06664210011318582</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -4362,6 +5111,9 @@
       <c r="D250">
         <v>5559201.188225526</v>
       </c>
+      <c r="E250">
+        <v>0.1552742406738911</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -4378,6 +5130,9 @@
       <c r="D251">
         <v>-223632.3814262059</v>
       </c>
+      <c r="E251">
+        <v>-0.02570487142829952</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -4394,6 +5149,9 @@
       <c r="D252">
         <v>-2463763.443200663</v>
       </c>
+      <c r="E252">
+        <v>-0.6315076830646296</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -4410,6 +5168,9 @@
       <c r="D253">
         <v>576657.5454394706</v>
       </c>
+      <c r="E253">
+        <v>0.1276921048360209</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -4426,6 +5187,9 @@
       <c r="D254">
         <v>1134688.971475951</v>
       </c>
+      <c r="E254">
+        <v>0.0825228342891601</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -4442,6 +5206,9 @@
       <c r="D255">
         <v>-734930.1402155887</v>
       </c>
+      <c r="E255">
+        <v>-0.1682520816513597</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -4458,6 +5225,9 @@
       <c r="D256">
         <v>-1258700.840215588</v>
       </c>
+      <c r="E256">
+        <v>-0.7318606821327666</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -4474,6 +5244,9 @@
       <c r="D257">
         <v>-465869.4039800996</v>
       </c>
+      <c r="E257">
+        <v>-0.2008057775776291</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -4490,6 +5263,9 @@
       <c r="D258">
         <v>-1936547.189635158</v>
       </c>
+      <c r="E258">
+        <v>-0.2420683987043947</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -4506,6 +5282,9 @@
       <c r="D259">
         <v>-945755.0134328362</v>
       </c>
+      <c r="E259">
+        <v>-0.4735314536539141</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -4522,6 +5301,9 @@
       <c r="D260">
         <v>-2015844.35</v>
       </c>
+      <c r="E260">
+        <v>-0.9980880138000281</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -4538,6 +5320,9 @@
       <c r="D261">
         <v>-25233.68167495821</v>
       </c>
+      <c r="E261">
+        <v>-0.003267341923469922</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -4554,6 +5339,9 @@
       <c r="D262">
         <v>13010030.68598673</v>
       </c>
+      <c r="E262">
+        <v>0.4437105150067499</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -4570,6 +5358,9 @@
       <c r="D263">
         <v>431209.5494195689</v>
       </c>
+      <c r="E263">
+        <v>0.03963177359468115</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -4586,6 +5377,9 @@
       <c r="D264">
         <v>-393848.3703980097</v>
       </c>
+      <c r="E264">
+        <v>-0.2188046502211165</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -4602,6 +5396,9 @@
       <c r="D265">
         <v>-571128.5289386385</v>
       </c>
+      <c r="E265">
+        <v>-0.192555909205081</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -4618,6 +5415,9 @@
       <c r="D266">
         <v>693502.7345771128</v>
       </c>
+      <c r="E266">
+        <v>0.1019414716523145</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -4634,6 +5434,9 @@
       <c r="D267">
         <v>130350.2178275287</v>
       </c>
+      <c r="E267">
+        <v>0.02607004356550574</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -4650,6 +5453,9 @@
       <c r="D268">
         <v>-190753.5642620237</v>
       </c>
+      <c r="E268">
+        <v>-0.1109120048224881</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -4666,6 +5472,9 @@
       <c r="D269">
         <v>89897.54519071244</v>
       </c>
+      <c r="E269">
+        <v>0.01775354195612493</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -4682,6 +5491,9 @@
       <c r="D270">
         <v>-80037.42470977455</v>
       </c>
+      <c r="E270">
+        <v>-0.002413526093239001</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -4698,6 +5510,9 @@
       <c r="D271">
         <v>-7604720.943864014</v>
       </c>
+      <c r="E271">
+        <v>-0.8561329676609672</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -4714,6 +5529,9 @@
       <c r="D272">
         <v>-1772871.417827534</v>
       </c>
+      <c r="E272">
+        <v>-0.1782527368583149</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -4730,6 +5548,9 @@
       <c r="D273">
         <v>333955.3131011608</v>
       </c>
+      <c r="E273">
+        <v>0.08522572862466078</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -4746,6 +5567,9 @@
       <c r="D274">
         <v>357955.351907131</v>
       </c>
+      <c r="E274">
+        <v>0.1478103793614171</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -4762,6 +5586,9 @@
       <c r="D275">
         <v>1965526.977197353</v>
       </c>
+      <c r="E275">
+        <v>0.05780069186955993</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -4778,6 +5605,9 @@
       <c r="D276">
         <v>4577373.675207296</v>
       </c>
+      <c r="E276">
+        <v>0.2674280826578777</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -4794,6 +5624,9 @@
       <c r="D277">
         <v>-3668547.938225538</v>
       </c>
+      <c r="E277">
+        <v>-1.816377204516667</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -4810,6 +5643,9 @@
       <c r="D278">
         <v>-10100842.63756219</v>
       </c>
+      <c r="E278">
+        <v>-3.006847490403357</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -4826,6 +5662,9 @@
       <c r="D279">
         <v>-4263301.178109448</v>
       </c>
+      <c r="E279">
+        <v>-0.2340672657356675</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -4842,6 +5681,9 @@
       <c r="D280">
         <v>4490640.975290217</v>
       </c>
+      <c r="E280">
+        <v>0.1327280431552908</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -4858,6 +5700,9 @@
       <c r="D281">
         <v>-4732332.480099499</v>
       </c>
+      <c r="E281">
+        <v>-0.5627699464977404</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -4874,6 +5719,9 @@
       <c r="D282">
         <v>-296688.3459369815</v>
       </c>
+      <c r="E282">
+        <v>-0.1041933028281082</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -4890,6 +5738,9 @@
       <c r="D283">
         <v>-1516726.608208954</v>
       </c>
+      <c r="E283">
+        <v>-0.4333504594882727</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -4906,6 +5757,9 @@
       <c r="D284">
         <v>-287440.0975953564</v>
       </c>
+      <c r="E284">
+        <v>-0.1423177915970723</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -4922,6 +5776,9 @@
       <c r="D285">
         <v>1532775.180016585</v>
       </c>
+      <c r="E285">
+        <v>0.1477373667485865</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -4938,6 +5795,9 @@
       <c r="D286">
         <v>-5100028.214510782</v>
       </c>
+      <c r="E286">
+        <v>-2.392239904925774</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -4954,6 +5814,9 @@
       <c r="D287">
         <v>-959796.4927031547</v>
       </c>
+      <c r="E287">
+        <v>-0.1703501442520557</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -4970,6 +5833,9 @@
       <c r="D288">
         <v>920990.9873963529</v>
       </c>
+      <c r="E288">
+        <v>0.1046580667495856</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -4986,6 +5852,9 @@
       <c r="D289">
         <v>943430.2109452747</v>
       </c>
+      <c r="E289">
+        <v>0.2190823615424248</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -5002,6 +5871,9 @@
       <c r="D290">
         <v>-2901042.343615249</v>
       </c>
+      <c r="E290">
+        <v>-0.1719136203623851</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -5018,6 +5890,9 @@
       <c r="D291">
         <v>-558738.2522388063</v>
       </c>
+      <c r="E291">
+        <v>-0.1862460840796021</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -5034,6 +5909,9 @@
       <c r="D292">
         <v>367743.9477611985</v>
       </c>
+      <c r="E292">
+        <v>0.03870988923802089</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -5050,6 +5928,9 @@
       <c r="D293">
         <v>2524992.70190713</v>
       </c>
+      <c r="E293">
+        <v>0.4794247763087016</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -5066,6 +5947,9 @@
       <c r="D294">
         <v>-281898.815008292</v>
       </c>
+      <c r="E294">
+        <v>-0.1001083529241925</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -5082,6 +5966,9 @@
       <c r="D295">
         <v>1374657.717993367</v>
       </c>
+      <c r="E295">
+        <v>0.1695211540462032</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -5098,6 +5985,9 @@
       <c r="D296">
         <v>649300.88358209</v>
       </c>
+      <c r="E296">
+        <v>0.07278509186480465</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -5114,6 +6004,9 @@
       <c r="D297">
         <v>495162.0133499149</v>
       </c>
+      <c r="E297">
+        <v>0.04060328493227988</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -5130,6 +6023,9 @@
       <c r="D298">
         <v>332944.2150082905</v>
       </c>
+      <c r="E298">
+        <v>0.04955380927372462</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -5146,6 +6042,9 @@
       <c r="D299">
         <v>-4222066.547844114</v>
       </c>
+      <c r="E299">
+        <v>-2.090436205984492</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -5162,6 +6061,9 @@
       <c r="D300">
         <v>5387934.46276949</v>
       </c>
+      <c r="E300">
+        <v>0.1749329371029055</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -5178,6 +6080,9 @@
       <c r="D301">
         <v>751288.5876451069</v>
       </c>
+      <c r="E301">
+        <v>0.08818245461112237</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -5194,6 +6099,9 @@
       <c r="D302">
         <v>619329.79726368</v>
       </c>
+      <c r="E302">
+        <v>0.07106480748866094</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -5210,6 +6118,9 @@
       <c r="D303">
         <v>-1473520.679850747</v>
       </c>
+      <c r="E303">
+        <v>-2.632311649625652</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -5226,6 +6137,9 @@
       <c r="D304">
         <v>-778510.7975953571</v>
       </c>
+      <c r="E304">
+        <v>-0.4865692484970982</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -5242,6 +6156,9 @@
       <c r="D305">
         <v>-354277.7833333337</v>
       </c>
+      <c r="E305">
+        <v>-0.20740522505044</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -5258,6 +6175,9 @@
       <c r="D306">
         <v>-1176703.618076285</v>
       </c>
+      <c r="E306">
+        <v>-0.2353407236152571</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -5274,6 +6194,9 @@
       <c r="D307">
         <v>-1658739.420149253</v>
       </c>
+      <c r="E307">
+        <v>-0.4947857143302349</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -5290,6 +6213,9 @@
       <c r="D308">
         <v>8054605.410945274</v>
       </c>
+      <c r="E308">
+        <v>0.4130566877407833</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -5306,6 +6232,9 @@
       <c r="D309">
         <v>2289093.543200663</v>
       </c>
+      <c r="E309">
+        <v>0.4569383711742284</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -5322,6 +6251,9 @@
       <c r="D310">
         <v>11014287.12180763</v>
       </c>
+      <c r="E310">
+        <v>0.4011707850605488</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -5338,6 +6270,9 @@
       <c r="D311">
         <v>6864852.743366499</v>
       </c>
+      <c r="E311">
+        <v>0.2056154666692575</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -5354,6 +6289,9 @@
       <c r="D312">
         <v>528766.8441127688</v>
       </c>
+      <c r="E312">
+        <v>0.08393124509726488</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -5370,6 +6308,9 @@
       <c r="D313">
         <v>1659577.258291874</v>
       </c>
+      <c r="E313">
+        <v>0.141713179924056</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -5386,6 +6327,9 @@
       <c r="D314">
         <v>5097823.718490876</v>
       </c>
+      <c r="E314">
+        <v>0.1415425202684036</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -5402,6 +6346,9 @@
       <c r="D315">
         <v>-1896458.031260365</v>
       </c>
+      <c r="E315">
+        <v>-0.4741145078150912</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -5418,6 +6365,9 @@
       <c r="D316">
         <v>3104324.421724718</v>
       </c>
+      <c r="E316">
+        <v>0.1724624678735955</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -5434,6 +6384,9 @@
       <c r="D317">
         <v>483362.6681592017</v>
       </c>
+      <c r="E317">
+        <v>0.07916268240377719</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -5450,6 +6403,9 @@
       <c r="D318">
         <v>-3180124.739386396</v>
       </c>
+      <c r="E318">
+        <v>-0.7041905977383518</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -5466,6 +6422,9 @@
       <c r="D319">
         <v>-1044050.06119403</v>
       </c>
+      <c r="E319">
+        <v>-0.2586025336369116</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -5482,6 +6441,9 @@
       <c r="D320">
         <v>-563100.8485903819</v>
       </c>
+      <c r="E320">
+        <v>-0.2059833664714681</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -5498,6 +6460,9 @@
       <c r="D321">
         <v>-8207968.651492536</v>
       </c>
+      <c r="E321">
+        <v>-1.967607384954587</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -5514,6 +6479,9 @@
       <c r="D322">
         <v>-2896396.50995025</v>
       </c>
+      <c r="E322">
+        <v>-0.1026112878911963</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -5530,6 +6498,9 @@
       <c r="D323">
         <v>-4896377.889137648</v>
       </c>
+      <c r="E323">
+        <v>-0.4075170005482785</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -5546,6 +6517,9 @@
       <c r="D324">
         <v>-2008615.810199005</v>
       </c>
+      <c r="E324">
+        <v>-0.9277671178748291</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -5562,6 +6536,9 @@
       <c r="D325">
         <v>2336575.332669984</v>
       </c>
+      <c r="E325">
+        <v>0.3025476282105378</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -5578,6 +6555,9 @@
       <c r="D326">
         <v>5959708.638225539</v>
       </c>
+      <c r="E326">
+        <v>0.460194946737208</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -5594,6 +6574,9 @@
       <c r="D327">
         <v>-1042537.904311774</v>
       </c>
+      <c r="E327">
+        <v>-0.2085075808623549</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -5610,6 +6593,9 @@
       <c r="D328">
         <v>-5126654.609121061</v>
       </c>
+      <c r="E328">
+        <v>-1.773028918926296</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -5626,6 +6612,9 @@
       <c r="D329">
         <v>2078569.659369826</v>
       </c>
+      <c r="E329">
+        <v>0.1144965109270588</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -5642,6 +6631,9 @@
       <c r="D330">
         <v>3866835.574212268</v>
       </c>
+      <c r="E330">
+        <v>0.2465808220840382</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -5658,6 +6650,9 @@
       <c r="D331">
         <v>-536603.860613599</v>
       </c>
+      <c r="E331">
+        <v>-0.2978205644639235</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -5674,6 +6669,9 @@
       <c r="D332">
         <v>-977830.391542288</v>
       </c>
+      <c r="E332">
+        <v>-0.3597292334533698</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -5690,6 +6688,9 @@
       <c r="D333">
         <v>-2298790.077114428</v>
       </c>
+      <c r="E333">
+        <v>-1.33661154435143</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -5706,6 +6707,9 @@
       <c r="D334">
         <v>-2123049.878358209</v>
       </c>
+      <c r="E334">
+        <v>-0.6641903382624115</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -5722,6 +6726,9 @@
       <c r="D335">
         <v>-4610522.272222228</v>
       </c>
+      <c r="E335">
+        <v>-0.1986846956649208</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -5738,6 +6745,9 @@
       <c r="D336">
         <v>-844115.671641791</v>
       </c>
+      <c r="E336">
+        <v>-0.753968889327167</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -5754,6 +6764,9 @@
       <c r="D337">
         <v>-2586363.965754554</v>
       </c>
+      <c r="E337">
+        <v>-0.1494343564884444</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -5770,6 +6783,9 @@
       <c r="D338">
         <v>-953059.7467661612</v>
       </c>
+      <c r="E338">
+        <v>-0.03114574335837128</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -5786,6 +6802,9 @@
       <c r="D339">
         <v>-297275.9096185728</v>
       </c>
+      <c r="E339">
+        <v>-0.1438488664238697</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -5802,6 +6821,9 @@
       <c r="D340">
         <v>-696410.6072139305</v>
       </c>
+      <c r="E340">
+        <v>-0.6764663498221247</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -5818,6 +6840,9 @@
       <c r="D341">
         <v>-2720304.917910447</v>
       </c>
+      <c r="E341">
+        <v>-1.34688163421332</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -5834,6 +6859,9 @@
       <c r="D342">
         <v>-1134414.913432836</v>
       </c>
+      <c r="E342">
+        <v>-0.432316166458147</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -5850,6 +6878,9 @@
       <c r="D343">
         <v>-4366381.752902152</v>
       </c>
+      <c r="E343">
+        <v>-0.3519856310279849</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -5866,6 +6897,9 @@
       <c r="D344">
         <v>-9368145.938971814</v>
       </c>
+      <c r="E344">
+        <v>-2.649152764761788</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -5882,6 +6916,9 @@
       <c r="D345">
         <v>-129880.7914593699</v>
       </c>
+      <c r="E345">
+        <v>-0.05304287815869065</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -5898,6 +6935,9 @@
       <c r="D346">
         <v>1812136.395190716</v>
       </c>
+      <c r="E346">
+        <v>0.1045966173270254</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -5914,6 +6954,9 @@
       <c r="D347">
         <v>3072714.248009949</v>
       </c>
+      <c r="E347">
+        <v>0.2997769998058487</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -5930,6 +6973,9 @@
       <c r="D348">
         <v>-895260.5027363189</v>
       </c>
+      <c r="E348">
+        <v>-0.4050879181989099</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -5946,6 +6992,9 @@
       <c r="D349">
         <v>-2539553.941873964</v>
       </c>
+      <c r="E349">
+        <v>-0.4022227409601134</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -5962,6 +7011,9 @@
       <c r="D350">
         <v>-471249.4892205647</v>
       </c>
+      <c r="E350">
+        <v>-0.1857389716141531</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -5978,6 +7030,9 @@
       <c r="D351">
         <v>8525459.786069639</v>
       </c>
+      <c r="E351">
+        <v>0.2249853005058199</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -5994,6 +7049,9 @@
       <c r="D352">
         <v>8530730.242122725</v>
       </c>
+      <c r="E352">
+        <v>0.2251243868622934</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -6010,6 +7068,9 @@
       <c r="D353">
         <v>-309220.9590381421</v>
       </c>
+      <c r="E353">
+        <v>-0.01282694341001512</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -6026,6 +7087,9 @@
       <c r="D354">
         <v>-406475.3140961868</v>
       </c>
+      <c r="E354">
+        <v>-0.2108388181189166</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -6042,6 +7106,9 @@
       <c r="D355">
         <v>-96808.01492537931</v>
       </c>
+      <c r="E355">
+        <v>-0.005140144958425315</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -6058,6 +7125,9 @@
       <c r="D356">
         <v>-1754552.945522387</v>
       </c>
+      <c r="E356">
+        <v>-0.8687170041196031</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -6074,6 +7144,9 @@
       <c r="D357">
         <v>-1271094.670149253</v>
       </c>
+      <c r="E357">
+        <v>-0.7054703850211946</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -6090,6 +7163,9 @@
       <c r="D358">
         <v>-6725387.363267001</v>
       </c>
+      <c r="E358">
+        <v>-3.329884331317034</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -6106,6 +7182,9 @@
       <c r="D359">
         <v>314146.8445273638</v>
       </c>
+      <c r="E359">
+        <v>0.033683179205895</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -6122,6 +7201,9 @@
       <c r="D360">
         <v>-115138.3371475963</v>
       </c>
+      <c r="E360">
+        <v>-0.02282781900525585</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -6138,6 +7220,9 @@
       <c r="D361">
         <v>-870867.3160862345</v>
       </c>
+      <c r="E361">
+        <v>-0.3534421484464985</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -6154,6 +7239,9 @@
       <c r="D362">
         <v>-2721259.577529022</v>
       </c>
+      <c r="E362">
+        <v>-0.5118074195647553</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -6170,6 +7258,9 @@
       <c r="D363">
         <v>-442835.896766169</v>
       </c>
+      <c r="E363">
+        <v>-0.1989165124901938</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -6186,6 +7277,9 @@
       <c r="D364">
         <v>27527.48756218934</v>
       </c>
+      <c r="E364">
+        <v>0.01137637694917868</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -6202,6 +7296,9 @@
       <c r="D365">
         <v>-3575274.340878936</v>
       </c>
+      <c r="E365">
+        <v>-0.6788435862897666</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -6218,6 +7315,9 @@
       <c r="D366">
         <v>-625071.6747097857</v>
       </c>
+      <c r="E366">
+        <v>-0.25711686769246</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -6234,6 +7334,9 @@
       <c r="D367">
         <v>-3390047.554975126</v>
       </c>
+      <c r="E367">
+        <v>-0.2339951337270419</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -6250,6 +7353,9 @@
       <c r="D368">
         <v>-963186.9476782791</v>
       </c>
+      <c r="E368">
+        <v>-0.1328152678511929</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -6266,6 +7372,9 @@
       <c r="D369">
         <v>478376.6020729644</v>
       </c>
+      <c r="E369">
+        <v>0.07359640031891761</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -6282,6 +7391,9 @@
       <c r="D370">
         <v>557679.793366503</v>
       </c>
+      <c r="E370">
+        <v>0.01710671064306333</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -6298,6 +7410,9 @@
       <c r="D371">
         <v>-256440.339054727</v>
       </c>
+      <c r="E371">
+        <v>-0.126969142565664</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -6314,6 +7429,9 @@
       <c r="D372">
         <v>-1128461.384411278</v>
       </c>
+      <c r="E372">
+        <v>-0.5587255691725816</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -6330,6 +7448,9 @@
       <c r="D373">
         <v>107989.4552238816</v>
       </c>
+      <c r="E373">
+        <v>0.03222834677024963</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -6346,6 +7467,9 @@
       <c r="D374">
         <v>1334778.152321723</v>
       </c>
+      <c r="E374">
+        <v>0.1539536152727212</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -6362,6 +7486,9 @@
       <c r="D375">
         <v>228823.3664179128</v>
       </c>
+      <c r="E375">
+        <v>0.02639253905799708</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -6378,6 +7505,9 @@
       <c r="D376">
         <v>-7411465.139054727</v>
       </c>
+      <c r="E376">
+        <v>-3.308453476115423</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -6394,6 +7524,9 @@
       <c r="D377">
         <v>2391980.235074627</v>
       </c>
+      <c r="E377">
+        <v>0.2715283625835623</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -6410,6 +7543,9 @@
       <c r="D378">
         <v>-53877.72238805983</v>
       </c>
+      <c r="E378">
+        <v>-0.006753727040125432</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -6426,6 +7562,9 @@
       <c r="D379">
         <v>10009566.49087894</v>
       </c>
+      <c r="E379">
+        <v>0.2315987086107303</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -6442,6 +7581,9 @@
       <c r="D380">
         <v>-1771256.182918741</v>
       </c>
+      <c r="E380">
+        <v>-0.8769871371965726</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -6458,6 +7600,9 @@
       <c r="D381">
         <v>-1907876.275124377</v>
       </c>
+      <c r="E381">
+        <v>-1.039093966287371</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -6474,6 +7619,9 @@
       <c r="D382">
         <v>1652218.495605305</v>
       </c>
+      <c r="E382">
+        <v>0.1573541424386005</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -6490,6 +7638,9 @@
       <c r="D383">
         <v>-906595.4902985077</v>
       </c>
+      <c r="E383">
+        <v>-0.4695729073308888</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -6506,6 +7657,9 @@
       <c r="D384">
         <v>-1164516.832006632</v>
       </c>
+      <c r="E384">
+        <v>-0.1711766541065387</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -6522,6 +7676,9 @@
       <c r="D385">
         <v>2724976.754726373</v>
       </c>
+      <c r="E385">
+        <v>0.07565975185406491</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -6538,6 +7695,9 @@
       <c r="D386">
         <v>9491784.664096186</v>
       </c>
+      <c r="E386">
+        <v>0.5114108116431134</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -6554,6 +7714,9 @@
       <c r="D387">
         <v>1546308.562189057</v>
       </c>
+      <c r="E387">
+        <v>0.1403884481537117</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -6570,6 +7733,9 @@
       <c r="D388">
         <v>-506419.9296849146</v>
       </c>
+      <c r="E388">
+        <v>-0.02414397757734993</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -6586,6 +7752,9 @@
       <c r="D389">
         <v>-386632.6817578771</v>
       </c>
+      <c r="E389">
+        <v>-0.3453424968115927</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -6602,6 +7771,9 @@
       <c r="D390">
         <v>-5809213.755887225</v>
       </c>
+      <c r="E390">
+        <v>-0.3763662945181228</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -6618,6 +7790,9 @@
       <c r="D391">
         <v>86309.78963515814</v>
       </c>
+      <c r="E391">
+        <v>0.01837160273204728</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -6634,6 +7809,9 @@
       <c r="D392">
         <v>8504639.777280264</v>
       </c>
+      <c r="E392">
+        <v>0.2084148716565889</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -6650,6 +7828,9 @@
       <c r="D393">
         <v>-5045506.565505803</v>
       </c>
+      <c r="E393">
+        <v>-0.8569281785414122</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -6666,6 +7847,9 @@
       <c r="D394">
         <v>754238.3296019901</v>
       </c>
+      <c r="E394">
+        <v>0.1189375717660764</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -6682,6 +7866,9 @@
       <c r="D395">
         <v>1012681.476119405</v>
       </c>
+      <c r="E395">
+        <v>0.09644585486851473</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
@@ -6698,6 +7885,9 @@
       <c r="D396">
         <v>-5568055.98225541</v>
       </c>
+      <c r="E396">
+        <v>-0.3006750152242418</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
@@ -6714,6 +7904,9 @@
       <c r="D397">
         <v>-30575.72222222295</v>
       </c>
+      <c r="E397">
+        <v>-0.005354882814852745</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
@@ -6730,6 +7923,9 @@
       <c r="D398">
         <v>-4584807.448839137</v>
       </c>
+      <c r="E398">
+        <v>-0.832281809356645</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
@@ -6746,6 +7942,9 @@
       <c r="D399">
         <v>392029.2865671646</v>
       </c>
+      <c r="E399">
+        <v>0.04900366082089557</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -6762,6 +7961,9 @@
       <c r="D400">
         <v>-715214.7249585409</v>
       </c>
+      <c r="E400">
+        <v>-0.3709820057505908</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -6778,6 +7980,9 @@
       <c r="D401">
         <v>-2512697.710447761</v>
       </c>
+      <c r="E401">
+        <v>-1.460986281733766</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -6794,6 +7999,9 @@
       <c r="D402">
         <v>1074626.178855722</v>
       </c>
+      <c r="E402">
+        <v>0.1773450997530699</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -6810,6 +8018,9 @@
       <c r="D403">
         <v>-4540203.899004975</v>
       </c>
+      <c r="E403">
+        <v>-2.247952869875603</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -6826,6 +8037,9 @@
       <c r="D404">
         <v>923922.2886401322</v>
       </c>
+      <c r="E404">
+        <v>0.1746082867747916</v>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
@@ -6842,6 +8056,9 @@
       <c r="D405">
         <v>286895.9859038163</v>
       </c>
+      <c r="E405">
+        <v>0.01702866505766479</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
@@ -6858,6 +8075,9 @@
       <c r="D406">
         <v>-1804891.880845771</v>
       </c>
+      <c r="E406">
+        <v>-0.769147324973673</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -6874,6 +8094,9 @@
       <c r="D407">
         <v>-1227351.38888889</v>
       </c>
+      <c r="E407">
+        <v>-0.607688143169793</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
@@ -6890,6 +8113,9 @@
       <c r="D408">
         <v>-515022.0474295197</v>
       </c>
+      <c r="E408">
+        <v>-0.2235804540136485</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
@@ -6906,6 +8132,9 @@
       <c r="D409">
         <v>305084.3076285217</v>
       </c>
+      <c r="E409">
+        <v>0.02508776710089581</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
@@ -6922,6 +8151,9 @@
       <c r="D410">
         <v>-1073195.778524048</v>
       </c>
+      <c r="E410">
+        <v>-0.4284830468746198</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
@@ -6938,6 +8170,9 @@
       <c r="D411">
         <v>-5595546.709286898</v>
       </c>
+      <c r="E411">
+        <v>-1.458792730183057</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
@@ -6954,6 +8189,9 @@
       <c r="D412">
         <v>-6106237.087562189</v>
       </c>
+      <c r="E412">
+        <v>-0.5495613433762104</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
@@ -6970,6 +8208,9 @@
       <c r="D413">
         <v>-4020175.489054721</v>
       </c>
+      <c r="E413">
+        <v>-0.2189978848590285</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
@@ -6986,6 +8227,9 @@
       <c r="D414">
         <v>-330838.8167495853</v>
       </c>
+      <c r="E414">
+        <v>-0.1028037191281929</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
@@ -7002,6 +8246,9 @@
       <c r="D415">
         <v>-687890.3961857366</v>
       </c>
+      <c r="E415">
+        <v>-0.3746483823208245</v>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
@@ -7018,6 +8265,9 @@
       <c r="D416">
         <v>13520032.63424544</v>
       </c>
+      <c r="E416">
+        <v>0.555685748229894</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
@@ -7034,6 +8284,9 @@
       <c r="D417">
         <v>2348106.091127692</v>
       </c>
+      <c r="E417">
+        <v>0.1892870690147273</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
@@ -7050,6 +8303,9 @@
       <c r="D418">
         <v>-4205439.722885573</v>
       </c>
+      <c r="E418">
+        <v>-0.9225125963843861</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
@@ -7066,6 +8322,9 @@
       <c r="D419">
         <v>-1109303.239635157</v>
       </c>
+      <c r="E419">
+        <v>-0.5546516198175785</v>
+      </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
@@ -7082,6 +8341,9 @@
       <c r="D420">
         <v>25221.55339966994</v>
       </c>
+      <c r="E420">
+        <v>0.004084462089015375</v>
+      </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
@@ -7098,6 +8360,9 @@
       <c r="D421">
         <v>-2327932.373631842</v>
       </c>
+      <c r="E421">
+        <v>-0.5956594340128964</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
@@ -7114,6 +8379,9 @@
       <c r="D422">
         <v>2750619.238640133</v>
       </c>
+      <c r="E422">
+        <v>0.2796515369228372</v>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
@@ -7130,6 +8398,9 @@
       <c r="D423">
         <v>3505717.39543947</v>
       </c>
+      <c r="E423">
+        <v>0.3029632204837855</v>
+      </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
@@ -7146,6 +8417,9 @@
       <c r="D424">
         <v>1351715.007960198</v>
       </c>
+      <c r="E424">
+        <v>0.2810101467631696</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
@@ -7162,6 +8436,9 @@
       <c r="D425">
         <v>7550996.384825859</v>
       </c>
+      <c r="E425">
+        <v>0.2220538412399809</v>
+      </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
@@ -7178,6 +8455,9 @@
       <c r="D426">
         <v>45238.96616915287</v>
       </c>
+      <c r="E426">
+        <v>0.02239878782810611</v>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
@@ -7194,6 +8474,9 @@
       <c r="D427">
         <v>6393828.244610281</v>
       </c>
+      <c r="E427">
+        <v>0.5275679606161903</v>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
@@ -7210,6 +8493,9 @@
       <c r="D428">
         <v>-1205586.556550581</v>
       </c>
+      <c r="E428">
+        <v>-0.4448906771375752</v>
+      </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
@@ -7226,6 +8512,9 @@
       <c r="D429">
         <v>15713.12396351621</v>
       </c>
+      <c r="E429">
+        <v>0.001917375234135161</v>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
@@ -7242,6 +8531,9 @@
       <c r="D430">
         <v>2081281.373880599</v>
       </c>
+      <c r="E430">
+        <v>0.2601601717350748</v>
+      </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
@@ -7258,6 +8550,9 @@
       <c r="D431">
         <v>4258246.007628515</v>
       </c>
+      <c r="E431">
+        <v>0.1062855088063243</v>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
@@ -7274,6 +8569,9 @@
       <c r="D432">
         <v>-766424.3223880595</v>
       </c>
+      <c r="E432">
+        <v>-0.2737229722814498</v>
+      </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
@@ -7290,6 +8588,9 @@
       <c r="D433">
         <v>-1858005.316169154</v>
       </c>
+      <c r="E433">
+        <v>-0.9199385040046194</v>
+      </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
@@ -7305,6 +8606,9 @@
       </c>
       <c r="D434">
         <v>-653068.9441127665</v>
+      </c>
+      <c r="E434">
+        <v>-0.05973191744116516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>